<commit_message>
Started working on particles
working on particles and edited the planning a little bit.
</commit_message>
<xml_diff>
--- a/Documents/AssetList-Planning.xlsx
+++ b/Documents/AssetList-Planning.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="425">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="430">
   <si>
     <t>Planning</t>
   </si>
@@ -1300,6 +1300,21 @@
   </si>
   <si>
     <t>7S-ENV-CombatMusic</t>
+  </si>
+  <si>
+    <t>Sea Ambient Sound</t>
+  </si>
+  <si>
+    <t>Bird Chirps</t>
+  </si>
+  <si>
+    <t>WeaponSpark</t>
+  </si>
+  <si>
+    <t>Butterflies</t>
+  </si>
+  <si>
+    <t>Floating Dust</t>
   </si>
 </sst>
 </file>
@@ -1845,8 +1860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BI93"/>
   <sheetViews>
-    <sheetView topLeftCell="L46" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="Q37" sqref="Q37"/>
+    <sheetView topLeftCell="A28" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="J47" sqref="J47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2529,7 +2544,7 @@
       <c r="B41" s="27"/>
       <c r="I41" s="27"/>
       <c r="J41" s="9" t="s">
-        <v>100</v>
+        <v>323</v>
       </c>
       <c r="M41" s="9" t="s">
         <v>322</v>
@@ -2588,10 +2603,10 @@
     <row r="44" spans="1:59" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B44" s="27"/>
       <c r="I44" s="27"/>
-      <c r="J44" s="9" t="s">
-        <v>323</v>
-      </c>
       <c r="P44" s="27"/>
+      <c r="Q44" s="9" t="s">
+        <v>100</v>
+      </c>
       <c r="W44" s="27"/>
       <c r="AD44" s="27"/>
       <c r="AK44" s="27"/>
@@ -3104,10 +3119,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:QF496"/>
+  <dimension ref="A1:QF504"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A300" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G309" sqref="G309"/>
+    <sheetView tabSelected="1" topLeftCell="A297" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I311" sqref="I311"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8383,355 +8398,1835 @@
       <c r="QE326" s="17"/>
       <c r="QF326" s="17"/>
     </row>
-    <row r="327" spans="1:448" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="328" spans="1:448" s="23" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A328" s="23" t="s">
+    <row r="327" spans="1:448" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A327" s="14" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="328" spans="1:448" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A328" s="17"/>
+      <c r="B328" s="17"/>
+      <c r="C328" s="17"/>
+      <c r="D328" s="17"/>
+      <c r="E328" s="17"/>
+      <c r="F328" s="17"/>
+      <c r="G328" s="17"/>
+      <c r="H328" s="17"/>
+      <c r="I328" s="17"/>
+      <c r="J328" s="17"/>
+      <c r="K328" s="17"/>
+      <c r="L328" s="17"/>
+      <c r="M328" s="17"/>
+      <c r="N328" s="17"/>
+      <c r="O328" s="17"/>
+      <c r="P328" s="17"/>
+      <c r="Q328" s="17"/>
+      <c r="R328" s="17"/>
+      <c r="S328" s="17"/>
+      <c r="T328" s="17"/>
+      <c r="U328" s="17"/>
+      <c r="V328" s="17"/>
+      <c r="W328" s="17"/>
+      <c r="X328" s="17"/>
+      <c r="Y328" s="17"/>
+      <c r="Z328" s="17"/>
+      <c r="AA328" s="17"/>
+      <c r="AB328" s="17"/>
+      <c r="AC328" s="17"/>
+      <c r="AD328" s="17"/>
+      <c r="AE328" s="17"/>
+      <c r="AF328" s="17"/>
+      <c r="AG328" s="17"/>
+      <c r="AH328" s="17"/>
+      <c r="AI328" s="17"/>
+      <c r="AJ328" s="17"/>
+      <c r="AK328" s="17"/>
+      <c r="AL328" s="17"/>
+      <c r="AM328" s="17"/>
+      <c r="AN328" s="17"/>
+      <c r="AO328" s="17"/>
+      <c r="AP328" s="17"/>
+      <c r="AQ328" s="17"/>
+      <c r="AR328" s="17"/>
+      <c r="AS328" s="17"/>
+      <c r="AT328" s="17"/>
+      <c r="AU328" s="17"/>
+      <c r="AV328" s="17"/>
+      <c r="AW328" s="17"/>
+      <c r="AX328" s="17"/>
+      <c r="AY328" s="17"/>
+      <c r="AZ328" s="17"/>
+      <c r="BA328" s="17"/>
+      <c r="BB328" s="17"/>
+      <c r="BC328" s="17"/>
+      <c r="BD328" s="17"/>
+      <c r="BE328" s="17"/>
+      <c r="BF328" s="17"/>
+      <c r="BG328" s="17"/>
+      <c r="BH328" s="17"/>
+      <c r="BI328" s="17"/>
+      <c r="BJ328" s="17"/>
+      <c r="BK328" s="17"/>
+      <c r="BL328" s="17"/>
+      <c r="BM328" s="17"/>
+      <c r="BN328" s="17"/>
+      <c r="BO328" s="17"/>
+      <c r="BP328" s="17"/>
+      <c r="BQ328" s="17"/>
+      <c r="BR328" s="17"/>
+      <c r="BS328" s="17"/>
+      <c r="BT328" s="17"/>
+      <c r="BU328" s="17"/>
+      <c r="BV328" s="17"/>
+      <c r="BW328" s="17"/>
+      <c r="BX328" s="17"/>
+      <c r="BY328" s="17"/>
+      <c r="BZ328" s="17"/>
+      <c r="CA328" s="17"/>
+      <c r="CB328" s="17"/>
+      <c r="CC328" s="17"/>
+      <c r="CD328" s="17"/>
+      <c r="CE328" s="17"/>
+      <c r="CF328" s="17"/>
+      <c r="CG328" s="17"/>
+      <c r="CH328" s="17"/>
+      <c r="CI328" s="17"/>
+      <c r="CJ328" s="17"/>
+      <c r="CK328" s="17"/>
+      <c r="CL328" s="17"/>
+      <c r="CM328" s="17"/>
+      <c r="CN328" s="17"/>
+      <c r="CO328" s="17"/>
+      <c r="CP328" s="17"/>
+      <c r="CQ328" s="17"/>
+      <c r="CR328" s="17"/>
+      <c r="CS328" s="17"/>
+      <c r="CT328" s="17"/>
+      <c r="CU328" s="17"/>
+      <c r="CV328" s="17"/>
+      <c r="CW328" s="17"/>
+      <c r="CX328" s="17"/>
+      <c r="CY328" s="17"/>
+      <c r="CZ328" s="17"/>
+      <c r="DA328" s="17"/>
+      <c r="DB328" s="17"/>
+      <c r="DC328" s="17"/>
+      <c r="DD328" s="17"/>
+      <c r="DE328" s="17"/>
+      <c r="DF328" s="17"/>
+      <c r="DG328" s="17"/>
+      <c r="DH328" s="17"/>
+      <c r="DI328" s="17"/>
+      <c r="DJ328" s="17"/>
+      <c r="DK328" s="17"/>
+      <c r="DL328" s="17"/>
+      <c r="DM328" s="17"/>
+      <c r="DN328" s="17"/>
+      <c r="DO328" s="17"/>
+      <c r="DP328" s="17"/>
+      <c r="DQ328" s="17"/>
+      <c r="DR328" s="17"/>
+      <c r="DS328" s="17"/>
+      <c r="DT328" s="17"/>
+      <c r="DU328" s="17"/>
+      <c r="DV328" s="17"/>
+      <c r="DW328" s="17"/>
+      <c r="DX328" s="17"/>
+      <c r="DY328" s="17"/>
+      <c r="DZ328" s="17"/>
+      <c r="EA328" s="17"/>
+      <c r="EB328" s="17"/>
+      <c r="EC328" s="17"/>
+      <c r="ED328" s="17"/>
+      <c r="EE328" s="17"/>
+      <c r="EF328" s="17"/>
+      <c r="EG328" s="17"/>
+      <c r="EH328" s="17"/>
+      <c r="EI328" s="17"/>
+      <c r="EJ328" s="17"/>
+      <c r="EK328" s="17"/>
+      <c r="EL328" s="17"/>
+      <c r="EM328" s="17"/>
+      <c r="EN328" s="17"/>
+      <c r="EO328" s="17"/>
+      <c r="EP328" s="17"/>
+      <c r="EQ328" s="17"/>
+      <c r="ER328" s="17"/>
+      <c r="ES328" s="17"/>
+      <c r="ET328" s="17"/>
+      <c r="EU328" s="17"/>
+      <c r="EV328" s="17"/>
+      <c r="EW328" s="17"/>
+      <c r="EX328" s="17"/>
+      <c r="EY328" s="17"/>
+      <c r="EZ328" s="17"/>
+      <c r="FA328" s="17"/>
+      <c r="FB328" s="17"/>
+      <c r="FC328" s="17"/>
+      <c r="FD328" s="17"/>
+      <c r="FE328" s="17"/>
+      <c r="FF328" s="17"/>
+      <c r="FG328" s="17"/>
+      <c r="FH328" s="17"/>
+      <c r="FI328" s="17"/>
+      <c r="FJ328" s="17"/>
+      <c r="FK328" s="17"/>
+      <c r="FL328" s="17"/>
+      <c r="FM328" s="17"/>
+      <c r="FN328" s="17"/>
+      <c r="FO328" s="17"/>
+      <c r="FP328" s="17"/>
+      <c r="FQ328" s="17"/>
+      <c r="FR328" s="17"/>
+      <c r="FS328" s="17"/>
+      <c r="FT328" s="17"/>
+      <c r="FU328" s="17"/>
+      <c r="FV328" s="17"/>
+      <c r="FW328" s="17"/>
+      <c r="FX328" s="17"/>
+      <c r="FY328" s="17"/>
+      <c r="FZ328" s="17"/>
+      <c r="GA328" s="17"/>
+      <c r="GB328" s="17"/>
+      <c r="GC328" s="17"/>
+      <c r="GD328" s="17"/>
+      <c r="GE328" s="17"/>
+      <c r="GF328" s="17"/>
+      <c r="GG328" s="17"/>
+      <c r="GH328" s="17"/>
+      <c r="GI328" s="17"/>
+      <c r="GJ328" s="17"/>
+      <c r="GK328" s="17"/>
+      <c r="GL328" s="17"/>
+      <c r="GM328" s="17"/>
+      <c r="GN328" s="17"/>
+      <c r="GO328" s="17"/>
+      <c r="GP328" s="17"/>
+      <c r="GQ328" s="17"/>
+      <c r="GR328" s="17"/>
+      <c r="GS328" s="17"/>
+      <c r="GT328" s="17"/>
+      <c r="GU328" s="17"/>
+      <c r="GV328" s="17"/>
+      <c r="GW328" s="17"/>
+      <c r="GX328" s="17"/>
+      <c r="GY328" s="17"/>
+      <c r="GZ328" s="17"/>
+      <c r="HA328" s="17"/>
+      <c r="HB328" s="17"/>
+      <c r="HC328" s="17"/>
+      <c r="HD328" s="17"/>
+      <c r="HE328" s="17"/>
+      <c r="HF328" s="17"/>
+      <c r="HG328" s="17"/>
+      <c r="HH328" s="17"/>
+      <c r="HI328" s="17"/>
+      <c r="HJ328" s="17"/>
+      <c r="HK328" s="17"/>
+      <c r="HL328" s="17"/>
+      <c r="HM328" s="17"/>
+      <c r="HN328" s="17"/>
+      <c r="HO328" s="17"/>
+      <c r="HP328" s="17"/>
+      <c r="HQ328" s="17"/>
+      <c r="HR328" s="17"/>
+      <c r="HS328" s="17"/>
+      <c r="HT328" s="17"/>
+      <c r="HU328" s="17"/>
+      <c r="HV328" s="17"/>
+      <c r="HW328" s="17"/>
+      <c r="HX328" s="17"/>
+      <c r="HY328" s="17"/>
+      <c r="HZ328" s="17"/>
+      <c r="IA328" s="17"/>
+      <c r="IB328" s="17"/>
+      <c r="IC328" s="17"/>
+      <c r="ID328" s="17"/>
+      <c r="IE328" s="17"/>
+      <c r="IF328" s="17"/>
+      <c r="IG328" s="17"/>
+      <c r="IH328" s="17"/>
+      <c r="II328" s="17"/>
+      <c r="IJ328" s="17"/>
+      <c r="IK328" s="17"/>
+      <c r="IL328" s="17"/>
+      <c r="IM328" s="17"/>
+      <c r="IN328" s="17"/>
+      <c r="IO328" s="17"/>
+      <c r="IP328" s="17"/>
+      <c r="IQ328" s="17"/>
+      <c r="IR328" s="17"/>
+      <c r="IS328" s="17"/>
+      <c r="IT328" s="17"/>
+      <c r="IU328" s="17"/>
+      <c r="IV328" s="17"/>
+      <c r="IW328" s="17"/>
+      <c r="IX328" s="17"/>
+      <c r="IY328" s="17"/>
+      <c r="IZ328" s="17"/>
+      <c r="JA328" s="17"/>
+      <c r="JB328" s="17"/>
+      <c r="JC328" s="17"/>
+      <c r="JD328" s="17"/>
+      <c r="JE328" s="17"/>
+      <c r="JF328" s="17"/>
+      <c r="JG328" s="17"/>
+      <c r="JH328" s="17"/>
+      <c r="JI328" s="17"/>
+      <c r="JJ328" s="17"/>
+      <c r="JK328" s="17"/>
+      <c r="JL328" s="17"/>
+      <c r="JM328" s="17"/>
+      <c r="JN328" s="17"/>
+      <c r="JO328" s="17"/>
+      <c r="JP328" s="17"/>
+      <c r="JQ328" s="17"/>
+      <c r="JR328" s="17"/>
+      <c r="JS328" s="17"/>
+      <c r="JT328" s="17"/>
+      <c r="JU328" s="17"/>
+      <c r="JV328" s="17"/>
+      <c r="JW328" s="17"/>
+      <c r="JX328" s="17"/>
+      <c r="JY328" s="17"/>
+      <c r="JZ328" s="17"/>
+      <c r="KA328" s="17"/>
+      <c r="KB328" s="17"/>
+      <c r="KC328" s="17"/>
+      <c r="KD328" s="17"/>
+      <c r="KE328" s="17"/>
+      <c r="KF328" s="17"/>
+      <c r="KG328" s="17"/>
+      <c r="KH328" s="17"/>
+      <c r="KI328" s="17"/>
+      <c r="KJ328" s="17"/>
+      <c r="KK328" s="17"/>
+      <c r="KL328" s="17"/>
+      <c r="KM328" s="17"/>
+      <c r="KN328" s="17"/>
+      <c r="KO328" s="17"/>
+      <c r="KP328" s="17"/>
+      <c r="KQ328" s="17"/>
+      <c r="KR328" s="17"/>
+      <c r="KS328" s="17"/>
+      <c r="KT328" s="17"/>
+      <c r="KU328" s="17"/>
+      <c r="KV328" s="17"/>
+      <c r="KW328" s="17"/>
+      <c r="KX328" s="17"/>
+      <c r="KY328" s="17"/>
+      <c r="KZ328" s="17"/>
+      <c r="LA328" s="17"/>
+      <c r="LB328" s="17"/>
+      <c r="LC328" s="17"/>
+      <c r="LD328" s="17"/>
+      <c r="LE328" s="17"/>
+      <c r="LF328" s="17"/>
+      <c r="LG328" s="17"/>
+      <c r="LH328" s="17"/>
+      <c r="LI328" s="17"/>
+      <c r="LJ328" s="17"/>
+      <c r="LK328" s="17"/>
+      <c r="LL328" s="17"/>
+      <c r="LM328" s="17"/>
+      <c r="LN328" s="17"/>
+      <c r="LO328" s="17"/>
+      <c r="LP328" s="17"/>
+      <c r="LQ328" s="17"/>
+      <c r="LR328" s="17"/>
+      <c r="LS328" s="17"/>
+      <c r="LT328" s="17"/>
+      <c r="LU328" s="17"/>
+      <c r="LV328" s="17"/>
+      <c r="LW328" s="17"/>
+      <c r="LX328" s="17"/>
+      <c r="LY328" s="17"/>
+      <c r="LZ328" s="17"/>
+      <c r="MA328" s="17"/>
+      <c r="MB328" s="17"/>
+      <c r="MC328" s="17"/>
+      <c r="MD328" s="17"/>
+      <c r="ME328" s="17"/>
+      <c r="MF328" s="17"/>
+      <c r="MG328" s="17"/>
+      <c r="MH328" s="17"/>
+      <c r="MI328" s="17"/>
+      <c r="MJ328" s="17"/>
+      <c r="MK328" s="17"/>
+      <c r="ML328" s="17"/>
+      <c r="MM328" s="17"/>
+      <c r="MN328" s="17"/>
+      <c r="MO328" s="17"/>
+      <c r="MP328" s="17"/>
+      <c r="MQ328" s="17"/>
+      <c r="MR328" s="17"/>
+      <c r="MS328" s="17"/>
+      <c r="MT328" s="17"/>
+      <c r="MU328" s="17"/>
+      <c r="MV328" s="17"/>
+      <c r="MW328" s="17"/>
+      <c r="MX328" s="17"/>
+      <c r="MY328" s="17"/>
+      <c r="MZ328" s="17"/>
+      <c r="NA328" s="17"/>
+      <c r="NB328" s="17"/>
+      <c r="NC328" s="17"/>
+      <c r="ND328" s="17"/>
+      <c r="NE328" s="17"/>
+      <c r="NF328" s="17"/>
+      <c r="NG328" s="17"/>
+      <c r="NH328" s="17"/>
+      <c r="NI328" s="17"/>
+      <c r="NJ328" s="17"/>
+      <c r="NK328" s="17"/>
+      <c r="NL328" s="17"/>
+      <c r="NM328" s="17"/>
+      <c r="NN328" s="17"/>
+      <c r="NO328" s="17"/>
+      <c r="NP328" s="17"/>
+      <c r="NQ328" s="17"/>
+      <c r="NR328" s="17"/>
+      <c r="NS328" s="17"/>
+      <c r="NT328" s="17"/>
+      <c r="NU328" s="17"/>
+      <c r="NV328" s="17"/>
+      <c r="NW328" s="17"/>
+      <c r="NX328" s="17"/>
+      <c r="NY328" s="17"/>
+      <c r="NZ328" s="17"/>
+      <c r="OA328" s="17"/>
+      <c r="OB328" s="17"/>
+      <c r="OC328" s="17"/>
+      <c r="OD328" s="17"/>
+      <c r="OE328" s="17"/>
+      <c r="OF328" s="17"/>
+      <c r="OG328" s="17"/>
+      <c r="OH328" s="17"/>
+      <c r="OI328" s="17"/>
+      <c r="OJ328" s="17"/>
+      <c r="OK328" s="17"/>
+      <c r="OL328" s="17"/>
+      <c r="OM328" s="17"/>
+      <c r="ON328" s="17"/>
+      <c r="OO328" s="17"/>
+      <c r="OP328" s="17"/>
+      <c r="OQ328" s="17"/>
+      <c r="OR328" s="17"/>
+      <c r="OS328" s="17"/>
+      <c r="OT328" s="17"/>
+      <c r="OU328" s="17"/>
+      <c r="OV328" s="17"/>
+      <c r="OW328" s="17"/>
+      <c r="OX328" s="17"/>
+      <c r="OY328" s="17"/>
+      <c r="OZ328" s="17"/>
+      <c r="PA328" s="17"/>
+      <c r="PB328" s="17"/>
+      <c r="PC328" s="17"/>
+      <c r="PD328" s="17"/>
+      <c r="PE328" s="17"/>
+      <c r="PF328" s="17"/>
+      <c r="PG328" s="17"/>
+      <c r="PH328" s="17"/>
+      <c r="PI328" s="17"/>
+      <c r="PJ328" s="17"/>
+      <c r="PK328" s="17"/>
+      <c r="PL328" s="17"/>
+      <c r="PM328" s="17"/>
+      <c r="PN328" s="17"/>
+      <c r="PO328" s="17"/>
+      <c r="PP328" s="17"/>
+      <c r="PQ328" s="17"/>
+      <c r="PR328" s="17"/>
+      <c r="PS328" s="17"/>
+      <c r="PT328" s="17"/>
+      <c r="PU328" s="17"/>
+      <c r="PV328" s="17"/>
+      <c r="PW328" s="17"/>
+      <c r="PX328" s="17"/>
+      <c r="PY328" s="17"/>
+      <c r="PZ328" s="17"/>
+      <c r="QA328" s="17"/>
+      <c r="QB328" s="17"/>
+      <c r="QC328" s="17"/>
+      <c r="QD328" s="17"/>
+      <c r="QE328" s="17"/>
+      <c r="QF328" s="17"/>
+    </row>
+    <row r="329" spans="1:448" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A329" s="14" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="330" spans="1:448" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A330" s="17"/>
+      <c r="B330" s="17"/>
+      <c r="C330" s="17"/>
+      <c r="D330" s="17"/>
+      <c r="E330" s="17"/>
+      <c r="F330" s="17"/>
+      <c r="G330" s="17"/>
+      <c r="H330" s="17"/>
+      <c r="I330" s="17"/>
+      <c r="J330" s="17"/>
+      <c r="K330" s="17"/>
+      <c r="L330" s="17"/>
+      <c r="M330" s="17"/>
+      <c r="N330" s="17"/>
+      <c r="O330" s="17"/>
+      <c r="P330" s="17"/>
+      <c r="Q330" s="17"/>
+      <c r="R330" s="17"/>
+      <c r="S330" s="17"/>
+      <c r="T330" s="17"/>
+      <c r="U330" s="17"/>
+      <c r="V330" s="17"/>
+      <c r="W330" s="17"/>
+      <c r="X330" s="17"/>
+      <c r="Y330" s="17"/>
+      <c r="Z330" s="17"/>
+      <c r="AA330" s="17"/>
+      <c r="AB330" s="17"/>
+      <c r="AC330" s="17"/>
+      <c r="AD330" s="17"/>
+      <c r="AE330" s="17"/>
+      <c r="AF330" s="17"/>
+      <c r="AG330" s="17"/>
+      <c r="AH330" s="17"/>
+      <c r="AI330" s="17"/>
+      <c r="AJ330" s="17"/>
+      <c r="AK330" s="17"/>
+      <c r="AL330" s="17"/>
+      <c r="AM330" s="17"/>
+      <c r="AN330" s="17"/>
+      <c r="AO330" s="17"/>
+      <c r="AP330" s="17"/>
+      <c r="AQ330" s="17"/>
+      <c r="AR330" s="17"/>
+      <c r="AS330" s="17"/>
+      <c r="AT330" s="17"/>
+      <c r="AU330" s="17"/>
+      <c r="AV330" s="17"/>
+      <c r="AW330" s="17"/>
+      <c r="AX330" s="17"/>
+      <c r="AY330" s="17"/>
+      <c r="AZ330" s="17"/>
+      <c r="BA330" s="17"/>
+      <c r="BB330" s="17"/>
+      <c r="BC330" s="17"/>
+      <c r="BD330" s="17"/>
+      <c r="BE330" s="17"/>
+      <c r="BF330" s="17"/>
+      <c r="BG330" s="17"/>
+      <c r="BH330" s="17"/>
+      <c r="BI330" s="17"/>
+      <c r="BJ330" s="17"/>
+      <c r="BK330" s="17"/>
+      <c r="BL330" s="17"/>
+      <c r="BM330" s="17"/>
+      <c r="BN330" s="17"/>
+      <c r="BO330" s="17"/>
+      <c r="BP330" s="17"/>
+      <c r="BQ330" s="17"/>
+      <c r="BR330" s="17"/>
+      <c r="BS330" s="17"/>
+      <c r="BT330" s="17"/>
+      <c r="BU330" s="17"/>
+      <c r="BV330" s="17"/>
+      <c r="BW330" s="17"/>
+      <c r="BX330" s="17"/>
+      <c r="BY330" s="17"/>
+      <c r="BZ330" s="17"/>
+      <c r="CA330" s="17"/>
+      <c r="CB330" s="17"/>
+      <c r="CC330" s="17"/>
+      <c r="CD330" s="17"/>
+      <c r="CE330" s="17"/>
+      <c r="CF330" s="17"/>
+      <c r="CG330" s="17"/>
+      <c r="CH330" s="17"/>
+      <c r="CI330" s="17"/>
+      <c r="CJ330" s="17"/>
+      <c r="CK330" s="17"/>
+      <c r="CL330" s="17"/>
+      <c r="CM330" s="17"/>
+      <c r="CN330" s="17"/>
+      <c r="CO330" s="17"/>
+      <c r="CP330" s="17"/>
+      <c r="CQ330" s="17"/>
+      <c r="CR330" s="17"/>
+      <c r="CS330" s="17"/>
+      <c r="CT330" s="17"/>
+      <c r="CU330" s="17"/>
+      <c r="CV330" s="17"/>
+      <c r="CW330" s="17"/>
+      <c r="CX330" s="17"/>
+      <c r="CY330" s="17"/>
+      <c r="CZ330" s="17"/>
+      <c r="DA330" s="17"/>
+      <c r="DB330" s="17"/>
+      <c r="DC330" s="17"/>
+      <c r="DD330" s="17"/>
+      <c r="DE330" s="17"/>
+      <c r="DF330" s="17"/>
+      <c r="DG330" s="17"/>
+      <c r="DH330" s="17"/>
+      <c r="DI330" s="17"/>
+      <c r="DJ330" s="17"/>
+      <c r="DK330" s="17"/>
+      <c r="DL330" s="17"/>
+      <c r="DM330" s="17"/>
+      <c r="DN330" s="17"/>
+      <c r="DO330" s="17"/>
+      <c r="DP330" s="17"/>
+      <c r="DQ330" s="17"/>
+      <c r="DR330" s="17"/>
+      <c r="DS330" s="17"/>
+      <c r="DT330" s="17"/>
+      <c r="DU330" s="17"/>
+      <c r="DV330" s="17"/>
+      <c r="DW330" s="17"/>
+      <c r="DX330" s="17"/>
+      <c r="DY330" s="17"/>
+      <c r="DZ330" s="17"/>
+      <c r="EA330" s="17"/>
+      <c r="EB330" s="17"/>
+      <c r="EC330" s="17"/>
+      <c r="ED330" s="17"/>
+      <c r="EE330" s="17"/>
+      <c r="EF330" s="17"/>
+      <c r="EG330" s="17"/>
+      <c r="EH330" s="17"/>
+      <c r="EI330" s="17"/>
+      <c r="EJ330" s="17"/>
+      <c r="EK330" s="17"/>
+      <c r="EL330" s="17"/>
+      <c r="EM330" s="17"/>
+      <c r="EN330" s="17"/>
+      <c r="EO330" s="17"/>
+      <c r="EP330" s="17"/>
+      <c r="EQ330" s="17"/>
+      <c r="ER330" s="17"/>
+      <c r="ES330" s="17"/>
+      <c r="ET330" s="17"/>
+      <c r="EU330" s="17"/>
+      <c r="EV330" s="17"/>
+      <c r="EW330" s="17"/>
+      <c r="EX330" s="17"/>
+      <c r="EY330" s="17"/>
+      <c r="EZ330" s="17"/>
+      <c r="FA330" s="17"/>
+      <c r="FB330" s="17"/>
+      <c r="FC330" s="17"/>
+      <c r="FD330" s="17"/>
+      <c r="FE330" s="17"/>
+      <c r="FF330" s="17"/>
+      <c r="FG330" s="17"/>
+      <c r="FH330" s="17"/>
+      <c r="FI330" s="17"/>
+      <c r="FJ330" s="17"/>
+      <c r="FK330" s="17"/>
+      <c r="FL330" s="17"/>
+      <c r="FM330" s="17"/>
+      <c r="FN330" s="17"/>
+      <c r="FO330" s="17"/>
+      <c r="FP330" s="17"/>
+      <c r="FQ330" s="17"/>
+      <c r="FR330" s="17"/>
+      <c r="FS330" s="17"/>
+      <c r="FT330" s="17"/>
+      <c r="FU330" s="17"/>
+      <c r="FV330" s="17"/>
+      <c r="FW330" s="17"/>
+      <c r="FX330" s="17"/>
+      <c r="FY330" s="17"/>
+      <c r="FZ330" s="17"/>
+      <c r="GA330" s="17"/>
+      <c r="GB330" s="17"/>
+      <c r="GC330" s="17"/>
+      <c r="GD330" s="17"/>
+      <c r="GE330" s="17"/>
+      <c r="GF330" s="17"/>
+      <c r="GG330" s="17"/>
+      <c r="GH330" s="17"/>
+      <c r="GI330" s="17"/>
+      <c r="GJ330" s="17"/>
+      <c r="GK330" s="17"/>
+      <c r="GL330" s="17"/>
+      <c r="GM330" s="17"/>
+      <c r="GN330" s="17"/>
+      <c r="GO330" s="17"/>
+      <c r="GP330" s="17"/>
+      <c r="GQ330" s="17"/>
+      <c r="GR330" s="17"/>
+      <c r="GS330" s="17"/>
+      <c r="GT330" s="17"/>
+      <c r="GU330" s="17"/>
+      <c r="GV330" s="17"/>
+      <c r="GW330" s="17"/>
+      <c r="GX330" s="17"/>
+      <c r="GY330" s="17"/>
+      <c r="GZ330" s="17"/>
+      <c r="HA330" s="17"/>
+      <c r="HB330" s="17"/>
+      <c r="HC330" s="17"/>
+      <c r="HD330" s="17"/>
+      <c r="HE330" s="17"/>
+      <c r="HF330" s="17"/>
+      <c r="HG330" s="17"/>
+      <c r="HH330" s="17"/>
+      <c r="HI330" s="17"/>
+      <c r="HJ330" s="17"/>
+      <c r="HK330" s="17"/>
+      <c r="HL330" s="17"/>
+      <c r="HM330" s="17"/>
+      <c r="HN330" s="17"/>
+      <c r="HO330" s="17"/>
+      <c r="HP330" s="17"/>
+      <c r="HQ330" s="17"/>
+      <c r="HR330" s="17"/>
+      <c r="HS330" s="17"/>
+      <c r="HT330" s="17"/>
+      <c r="HU330" s="17"/>
+      <c r="HV330" s="17"/>
+      <c r="HW330" s="17"/>
+      <c r="HX330" s="17"/>
+      <c r="HY330" s="17"/>
+      <c r="HZ330" s="17"/>
+      <c r="IA330" s="17"/>
+      <c r="IB330" s="17"/>
+      <c r="IC330" s="17"/>
+      <c r="ID330" s="17"/>
+      <c r="IE330" s="17"/>
+      <c r="IF330" s="17"/>
+      <c r="IG330" s="17"/>
+      <c r="IH330" s="17"/>
+      <c r="II330" s="17"/>
+      <c r="IJ330" s="17"/>
+      <c r="IK330" s="17"/>
+      <c r="IL330" s="17"/>
+      <c r="IM330" s="17"/>
+      <c r="IN330" s="17"/>
+      <c r="IO330" s="17"/>
+      <c r="IP330" s="17"/>
+      <c r="IQ330" s="17"/>
+      <c r="IR330" s="17"/>
+      <c r="IS330" s="17"/>
+      <c r="IT330" s="17"/>
+      <c r="IU330" s="17"/>
+      <c r="IV330" s="17"/>
+      <c r="IW330" s="17"/>
+      <c r="IX330" s="17"/>
+      <c r="IY330" s="17"/>
+      <c r="IZ330" s="17"/>
+      <c r="JA330" s="17"/>
+      <c r="JB330" s="17"/>
+      <c r="JC330" s="17"/>
+      <c r="JD330" s="17"/>
+      <c r="JE330" s="17"/>
+      <c r="JF330" s="17"/>
+      <c r="JG330" s="17"/>
+      <c r="JH330" s="17"/>
+      <c r="JI330" s="17"/>
+      <c r="JJ330" s="17"/>
+      <c r="JK330" s="17"/>
+      <c r="JL330" s="17"/>
+      <c r="JM330" s="17"/>
+      <c r="JN330" s="17"/>
+      <c r="JO330" s="17"/>
+      <c r="JP330" s="17"/>
+      <c r="JQ330" s="17"/>
+      <c r="JR330" s="17"/>
+      <c r="JS330" s="17"/>
+      <c r="JT330" s="17"/>
+      <c r="JU330" s="17"/>
+      <c r="JV330" s="17"/>
+      <c r="JW330" s="17"/>
+      <c r="JX330" s="17"/>
+      <c r="JY330" s="17"/>
+      <c r="JZ330" s="17"/>
+      <c r="KA330" s="17"/>
+      <c r="KB330" s="17"/>
+      <c r="KC330" s="17"/>
+      <c r="KD330" s="17"/>
+      <c r="KE330" s="17"/>
+      <c r="KF330" s="17"/>
+      <c r="KG330" s="17"/>
+      <c r="KH330" s="17"/>
+      <c r="KI330" s="17"/>
+      <c r="KJ330" s="17"/>
+      <c r="KK330" s="17"/>
+      <c r="KL330" s="17"/>
+      <c r="KM330" s="17"/>
+      <c r="KN330" s="17"/>
+      <c r="KO330" s="17"/>
+      <c r="KP330" s="17"/>
+      <c r="KQ330" s="17"/>
+      <c r="KR330" s="17"/>
+      <c r="KS330" s="17"/>
+      <c r="KT330" s="17"/>
+      <c r="KU330" s="17"/>
+      <c r="KV330" s="17"/>
+      <c r="KW330" s="17"/>
+      <c r="KX330" s="17"/>
+      <c r="KY330" s="17"/>
+      <c r="KZ330" s="17"/>
+      <c r="LA330" s="17"/>
+      <c r="LB330" s="17"/>
+      <c r="LC330" s="17"/>
+      <c r="LD330" s="17"/>
+      <c r="LE330" s="17"/>
+      <c r="LF330" s="17"/>
+      <c r="LG330" s="17"/>
+      <c r="LH330" s="17"/>
+      <c r="LI330" s="17"/>
+      <c r="LJ330" s="17"/>
+      <c r="LK330" s="17"/>
+      <c r="LL330" s="17"/>
+      <c r="LM330" s="17"/>
+      <c r="LN330" s="17"/>
+      <c r="LO330" s="17"/>
+      <c r="LP330" s="17"/>
+      <c r="LQ330" s="17"/>
+      <c r="LR330" s="17"/>
+      <c r="LS330" s="17"/>
+      <c r="LT330" s="17"/>
+      <c r="LU330" s="17"/>
+      <c r="LV330" s="17"/>
+      <c r="LW330" s="17"/>
+      <c r="LX330" s="17"/>
+      <c r="LY330" s="17"/>
+      <c r="LZ330" s="17"/>
+      <c r="MA330" s="17"/>
+      <c r="MB330" s="17"/>
+      <c r="MC330" s="17"/>
+      <c r="MD330" s="17"/>
+      <c r="ME330" s="17"/>
+      <c r="MF330" s="17"/>
+      <c r="MG330" s="17"/>
+      <c r="MH330" s="17"/>
+      <c r="MI330" s="17"/>
+      <c r="MJ330" s="17"/>
+      <c r="MK330" s="17"/>
+      <c r="ML330" s="17"/>
+      <c r="MM330" s="17"/>
+      <c r="MN330" s="17"/>
+      <c r="MO330" s="17"/>
+      <c r="MP330" s="17"/>
+      <c r="MQ330" s="17"/>
+      <c r="MR330" s="17"/>
+      <c r="MS330" s="17"/>
+      <c r="MT330" s="17"/>
+      <c r="MU330" s="17"/>
+      <c r="MV330" s="17"/>
+      <c r="MW330" s="17"/>
+      <c r="MX330" s="17"/>
+      <c r="MY330" s="17"/>
+      <c r="MZ330" s="17"/>
+      <c r="NA330" s="17"/>
+      <c r="NB330" s="17"/>
+      <c r="NC330" s="17"/>
+      <c r="ND330" s="17"/>
+      <c r="NE330" s="17"/>
+      <c r="NF330" s="17"/>
+      <c r="NG330" s="17"/>
+      <c r="NH330" s="17"/>
+      <c r="NI330" s="17"/>
+      <c r="NJ330" s="17"/>
+      <c r="NK330" s="17"/>
+      <c r="NL330" s="17"/>
+      <c r="NM330" s="17"/>
+      <c r="NN330" s="17"/>
+      <c r="NO330" s="17"/>
+      <c r="NP330" s="17"/>
+      <c r="NQ330" s="17"/>
+      <c r="NR330" s="17"/>
+      <c r="NS330" s="17"/>
+      <c r="NT330" s="17"/>
+      <c r="NU330" s="17"/>
+      <c r="NV330" s="17"/>
+      <c r="NW330" s="17"/>
+      <c r="NX330" s="17"/>
+      <c r="NY330" s="17"/>
+      <c r="NZ330" s="17"/>
+      <c r="OA330" s="17"/>
+      <c r="OB330" s="17"/>
+      <c r="OC330" s="17"/>
+      <c r="OD330" s="17"/>
+      <c r="OE330" s="17"/>
+      <c r="OF330" s="17"/>
+      <c r="OG330" s="17"/>
+      <c r="OH330" s="17"/>
+      <c r="OI330" s="17"/>
+      <c r="OJ330" s="17"/>
+      <c r="OK330" s="17"/>
+      <c r="OL330" s="17"/>
+      <c r="OM330" s="17"/>
+      <c r="ON330" s="17"/>
+      <c r="OO330" s="17"/>
+      <c r="OP330" s="17"/>
+      <c r="OQ330" s="17"/>
+      <c r="OR330" s="17"/>
+      <c r="OS330" s="17"/>
+      <c r="OT330" s="17"/>
+      <c r="OU330" s="17"/>
+      <c r="OV330" s="17"/>
+      <c r="OW330" s="17"/>
+      <c r="OX330" s="17"/>
+      <c r="OY330" s="17"/>
+      <c r="OZ330" s="17"/>
+      <c r="PA330" s="17"/>
+      <c r="PB330" s="17"/>
+      <c r="PC330" s="17"/>
+      <c r="PD330" s="17"/>
+      <c r="PE330" s="17"/>
+      <c r="PF330" s="17"/>
+      <c r="PG330" s="17"/>
+      <c r="PH330" s="17"/>
+      <c r="PI330" s="17"/>
+      <c r="PJ330" s="17"/>
+      <c r="PK330" s="17"/>
+      <c r="PL330" s="17"/>
+      <c r="PM330" s="17"/>
+      <c r="PN330" s="17"/>
+      <c r="PO330" s="17"/>
+      <c r="PP330" s="17"/>
+      <c r="PQ330" s="17"/>
+      <c r="PR330" s="17"/>
+      <c r="PS330" s="17"/>
+      <c r="PT330" s="17"/>
+      <c r="PU330" s="17"/>
+      <c r="PV330" s="17"/>
+      <c r="PW330" s="17"/>
+      <c r="PX330" s="17"/>
+      <c r="PY330" s="17"/>
+      <c r="PZ330" s="17"/>
+      <c r="QA330" s="17"/>
+      <c r="QB330" s="17"/>
+      <c r="QC330" s="17"/>
+      <c r="QD330" s="17"/>
+      <c r="QE330" s="17"/>
+      <c r="QF330" s="17"/>
+    </row>
+    <row r="331" spans="1:448" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A331" s="14" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="332" spans="1:448" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A332" s="17"/>
+      <c r="B332" s="17"/>
+      <c r="C332" s="17"/>
+      <c r="D332" s="17"/>
+      <c r="E332" s="17"/>
+      <c r="F332" s="17"/>
+      <c r="G332" s="17"/>
+      <c r="H332" s="17"/>
+      <c r="I332" s="17"/>
+      <c r="J332" s="17"/>
+      <c r="K332" s="17"/>
+      <c r="L332" s="17"/>
+      <c r="M332" s="17"/>
+      <c r="N332" s="17"/>
+      <c r="O332" s="17"/>
+      <c r="P332" s="17"/>
+      <c r="Q332" s="17"/>
+      <c r="R332" s="17"/>
+      <c r="S332" s="17"/>
+      <c r="T332" s="17"/>
+      <c r="U332" s="17"/>
+      <c r="V332" s="17"/>
+      <c r="W332" s="17"/>
+      <c r="X332" s="17"/>
+      <c r="Y332" s="17"/>
+      <c r="Z332" s="17"/>
+      <c r="AA332" s="17"/>
+      <c r="AB332" s="17"/>
+      <c r="AC332" s="17"/>
+      <c r="AD332" s="17"/>
+      <c r="AE332" s="17"/>
+      <c r="AF332" s="17"/>
+      <c r="AG332" s="17"/>
+      <c r="AH332" s="17"/>
+      <c r="AI332" s="17"/>
+      <c r="AJ332" s="17"/>
+      <c r="AK332" s="17"/>
+      <c r="AL332" s="17"/>
+      <c r="AM332" s="17"/>
+      <c r="AN332" s="17"/>
+      <c r="AO332" s="17"/>
+      <c r="AP332" s="17"/>
+      <c r="AQ332" s="17"/>
+      <c r="AR332" s="17"/>
+      <c r="AS332" s="17"/>
+      <c r="AT332" s="17"/>
+      <c r="AU332" s="17"/>
+      <c r="AV332" s="17"/>
+      <c r="AW332" s="17"/>
+      <c r="AX332" s="17"/>
+      <c r="AY332" s="17"/>
+      <c r="AZ332" s="17"/>
+      <c r="BA332" s="17"/>
+      <c r="BB332" s="17"/>
+      <c r="BC332" s="17"/>
+      <c r="BD332" s="17"/>
+      <c r="BE332" s="17"/>
+      <c r="BF332" s="17"/>
+      <c r="BG332" s="17"/>
+      <c r="BH332" s="17"/>
+      <c r="BI332" s="17"/>
+      <c r="BJ332" s="17"/>
+      <c r="BK332" s="17"/>
+      <c r="BL332" s="17"/>
+      <c r="BM332" s="17"/>
+      <c r="BN332" s="17"/>
+      <c r="BO332" s="17"/>
+      <c r="BP332" s="17"/>
+      <c r="BQ332" s="17"/>
+      <c r="BR332" s="17"/>
+      <c r="BS332" s="17"/>
+      <c r="BT332" s="17"/>
+      <c r="BU332" s="17"/>
+      <c r="BV332" s="17"/>
+      <c r="BW332" s="17"/>
+      <c r="BX332" s="17"/>
+      <c r="BY332" s="17"/>
+      <c r="BZ332" s="17"/>
+      <c r="CA332" s="17"/>
+      <c r="CB332" s="17"/>
+      <c r="CC332" s="17"/>
+      <c r="CD332" s="17"/>
+      <c r="CE332" s="17"/>
+      <c r="CF332" s="17"/>
+      <c r="CG332" s="17"/>
+      <c r="CH332" s="17"/>
+      <c r="CI332" s="17"/>
+      <c r="CJ332" s="17"/>
+      <c r="CK332" s="17"/>
+      <c r="CL332" s="17"/>
+      <c r="CM332" s="17"/>
+      <c r="CN332" s="17"/>
+      <c r="CO332" s="17"/>
+      <c r="CP332" s="17"/>
+      <c r="CQ332" s="17"/>
+      <c r="CR332" s="17"/>
+      <c r="CS332" s="17"/>
+      <c r="CT332" s="17"/>
+      <c r="CU332" s="17"/>
+      <c r="CV332" s="17"/>
+      <c r="CW332" s="17"/>
+      <c r="CX332" s="17"/>
+      <c r="CY332" s="17"/>
+      <c r="CZ332" s="17"/>
+      <c r="DA332" s="17"/>
+      <c r="DB332" s="17"/>
+      <c r="DC332" s="17"/>
+      <c r="DD332" s="17"/>
+      <c r="DE332" s="17"/>
+      <c r="DF332" s="17"/>
+      <c r="DG332" s="17"/>
+      <c r="DH332" s="17"/>
+      <c r="DI332" s="17"/>
+      <c r="DJ332" s="17"/>
+      <c r="DK332" s="17"/>
+      <c r="DL332" s="17"/>
+      <c r="DM332" s="17"/>
+      <c r="DN332" s="17"/>
+      <c r="DO332" s="17"/>
+      <c r="DP332" s="17"/>
+      <c r="DQ332" s="17"/>
+      <c r="DR332" s="17"/>
+      <c r="DS332" s="17"/>
+      <c r="DT332" s="17"/>
+      <c r="DU332" s="17"/>
+      <c r="DV332" s="17"/>
+      <c r="DW332" s="17"/>
+      <c r="DX332" s="17"/>
+      <c r="DY332" s="17"/>
+      <c r="DZ332" s="17"/>
+      <c r="EA332" s="17"/>
+      <c r="EB332" s="17"/>
+      <c r="EC332" s="17"/>
+      <c r="ED332" s="17"/>
+      <c r="EE332" s="17"/>
+      <c r="EF332" s="17"/>
+      <c r="EG332" s="17"/>
+      <c r="EH332" s="17"/>
+      <c r="EI332" s="17"/>
+      <c r="EJ332" s="17"/>
+      <c r="EK332" s="17"/>
+      <c r="EL332" s="17"/>
+      <c r="EM332" s="17"/>
+      <c r="EN332" s="17"/>
+      <c r="EO332" s="17"/>
+      <c r="EP332" s="17"/>
+      <c r="EQ332" s="17"/>
+      <c r="ER332" s="17"/>
+      <c r="ES332" s="17"/>
+      <c r="ET332" s="17"/>
+      <c r="EU332" s="17"/>
+      <c r="EV332" s="17"/>
+      <c r="EW332" s="17"/>
+      <c r="EX332" s="17"/>
+      <c r="EY332" s="17"/>
+      <c r="EZ332" s="17"/>
+      <c r="FA332" s="17"/>
+      <c r="FB332" s="17"/>
+      <c r="FC332" s="17"/>
+      <c r="FD332" s="17"/>
+      <c r="FE332" s="17"/>
+      <c r="FF332" s="17"/>
+      <c r="FG332" s="17"/>
+      <c r="FH332" s="17"/>
+      <c r="FI332" s="17"/>
+      <c r="FJ332" s="17"/>
+      <c r="FK332" s="17"/>
+      <c r="FL332" s="17"/>
+      <c r="FM332" s="17"/>
+      <c r="FN332" s="17"/>
+      <c r="FO332" s="17"/>
+      <c r="FP332" s="17"/>
+      <c r="FQ332" s="17"/>
+      <c r="FR332" s="17"/>
+      <c r="FS332" s="17"/>
+      <c r="FT332" s="17"/>
+      <c r="FU332" s="17"/>
+      <c r="FV332" s="17"/>
+      <c r="FW332" s="17"/>
+      <c r="FX332" s="17"/>
+      <c r="FY332" s="17"/>
+      <c r="FZ332" s="17"/>
+      <c r="GA332" s="17"/>
+      <c r="GB332" s="17"/>
+      <c r="GC332" s="17"/>
+      <c r="GD332" s="17"/>
+      <c r="GE332" s="17"/>
+      <c r="GF332" s="17"/>
+      <c r="GG332" s="17"/>
+      <c r="GH332" s="17"/>
+      <c r="GI332" s="17"/>
+      <c r="GJ332" s="17"/>
+      <c r="GK332" s="17"/>
+      <c r="GL332" s="17"/>
+      <c r="GM332" s="17"/>
+      <c r="GN332" s="17"/>
+      <c r="GO332" s="17"/>
+      <c r="GP332" s="17"/>
+      <c r="GQ332" s="17"/>
+      <c r="GR332" s="17"/>
+      <c r="GS332" s="17"/>
+      <c r="GT332" s="17"/>
+      <c r="GU332" s="17"/>
+      <c r="GV332" s="17"/>
+      <c r="GW332" s="17"/>
+      <c r="GX332" s="17"/>
+      <c r="GY332" s="17"/>
+      <c r="GZ332" s="17"/>
+      <c r="HA332" s="17"/>
+      <c r="HB332" s="17"/>
+      <c r="HC332" s="17"/>
+      <c r="HD332" s="17"/>
+      <c r="HE332" s="17"/>
+      <c r="HF332" s="17"/>
+      <c r="HG332" s="17"/>
+      <c r="HH332" s="17"/>
+      <c r="HI332" s="17"/>
+      <c r="HJ332" s="17"/>
+      <c r="HK332" s="17"/>
+      <c r="HL332" s="17"/>
+      <c r="HM332" s="17"/>
+      <c r="HN332" s="17"/>
+      <c r="HO332" s="17"/>
+      <c r="HP332" s="17"/>
+      <c r="HQ332" s="17"/>
+      <c r="HR332" s="17"/>
+      <c r="HS332" s="17"/>
+      <c r="HT332" s="17"/>
+      <c r="HU332" s="17"/>
+      <c r="HV332" s="17"/>
+      <c r="HW332" s="17"/>
+      <c r="HX332" s="17"/>
+      <c r="HY332" s="17"/>
+      <c r="HZ332" s="17"/>
+      <c r="IA332" s="17"/>
+      <c r="IB332" s="17"/>
+      <c r="IC332" s="17"/>
+      <c r="ID332" s="17"/>
+      <c r="IE332" s="17"/>
+      <c r="IF332" s="17"/>
+      <c r="IG332" s="17"/>
+      <c r="IH332" s="17"/>
+      <c r="II332" s="17"/>
+      <c r="IJ332" s="17"/>
+      <c r="IK332" s="17"/>
+      <c r="IL332" s="17"/>
+      <c r="IM332" s="17"/>
+      <c r="IN332" s="17"/>
+      <c r="IO332" s="17"/>
+      <c r="IP332" s="17"/>
+      <c r="IQ332" s="17"/>
+      <c r="IR332" s="17"/>
+      <c r="IS332" s="17"/>
+      <c r="IT332" s="17"/>
+      <c r="IU332" s="17"/>
+      <c r="IV332" s="17"/>
+      <c r="IW332" s="17"/>
+      <c r="IX332" s="17"/>
+      <c r="IY332" s="17"/>
+      <c r="IZ332" s="17"/>
+      <c r="JA332" s="17"/>
+      <c r="JB332" s="17"/>
+      <c r="JC332" s="17"/>
+      <c r="JD332" s="17"/>
+      <c r="JE332" s="17"/>
+      <c r="JF332" s="17"/>
+      <c r="JG332" s="17"/>
+      <c r="JH332" s="17"/>
+      <c r="JI332" s="17"/>
+      <c r="JJ332" s="17"/>
+      <c r="JK332" s="17"/>
+      <c r="JL332" s="17"/>
+      <c r="JM332" s="17"/>
+      <c r="JN332" s="17"/>
+      <c r="JO332" s="17"/>
+      <c r="JP332" s="17"/>
+      <c r="JQ332" s="17"/>
+      <c r="JR332" s="17"/>
+      <c r="JS332" s="17"/>
+      <c r="JT332" s="17"/>
+      <c r="JU332" s="17"/>
+      <c r="JV332" s="17"/>
+      <c r="JW332" s="17"/>
+      <c r="JX332" s="17"/>
+      <c r="JY332" s="17"/>
+      <c r="JZ332" s="17"/>
+      <c r="KA332" s="17"/>
+      <c r="KB332" s="17"/>
+      <c r="KC332" s="17"/>
+      <c r="KD332" s="17"/>
+      <c r="KE332" s="17"/>
+      <c r="KF332" s="17"/>
+      <c r="KG332" s="17"/>
+      <c r="KH332" s="17"/>
+      <c r="KI332" s="17"/>
+      <c r="KJ332" s="17"/>
+      <c r="KK332" s="17"/>
+      <c r="KL332" s="17"/>
+      <c r="KM332" s="17"/>
+      <c r="KN332" s="17"/>
+      <c r="KO332" s="17"/>
+      <c r="KP332" s="17"/>
+      <c r="KQ332" s="17"/>
+      <c r="KR332" s="17"/>
+      <c r="KS332" s="17"/>
+      <c r="KT332" s="17"/>
+      <c r="KU332" s="17"/>
+      <c r="KV332" s="17"/>
+      <c r="KW332" s="17"/>
+      <c r="KX332" s="17"/>
+      <c r="KY332" s="17"/>
+      <c r="KZ332" s="17"/>
+      <c r="LA332" s="17"/>
+      <c r="LB332" s="17"/>
+      <c r="LC332" s="17"/>
+      <c r="LD332" s="17"/>
+      <c r="LE332" s="17"/>
+      <c r="LF332" s="17"/>
+      <c r="LG332" s="17"/>
+      <c r="LH332" s="17"/>
+      <c r="LI332" s="17"/>
+      <c r="LJ332" s="17"/>
+      <c r="LK332" s="17"/>
+      <c r="LL332" s="17"/>
+      <c r="LM332" s="17"/>
+      <c r="LN332" s="17"/>
+      <c r="LO332" s="17"/>
+      <c r="LP332" s="17"/>
+      <c r="LQ332" s="17"/>
+      <c r="LR332" s="17"/>
+      <c r="LS332" s="17"/>
+      <c r="LT332" s="17"/>
+      <c r="LU332" s="17"/>
+      <c r="LV332" s="17"/>
+      <c r="LW332" s="17"/>
+      <c r="LX332" s="17"/>
+      <c r="LY332" s="17"/>
+      <c r="LZ332" s="17"/>
+      <c r="MA332" s="17"/>
+      <c r="MB332" s="17"/>
+      <c r="MC332" s="17"/>
+      <c r="MD332" s="17"/>
+      <c r="ME332" s="17"/>
+      <c r="MF332" s="17"/>
+      <c r="MG332" s="17"/>
+      <c r="MH332" s="17"/>
+      <c r="MI332" s="17"/>
+      <c r="MJ332" s="17"/>
+      <c r="MK332" s="17"/>
+      <c r="ML332" s="17"/>
+      <c r="MM332" s="17"/>
+      <c r="MN332" s="17"/>
+      <c r="MO332" s="17"/>
+      <c r="MP332" s="17"/>
+      <c r="MQ332" s="17"/>
+      <c r="MR332" s="17"/>
+      <c r="MS332" s="17"/>
+      <c r="MT332" s="17"/>
+      <c r="MU332" s="17"/>
+      <c r="MV332" s="17"/>
+      <c r="MW332" s="17"/>
+      <c r="MX332" s="17"/>
+      <c r="MY332" s="17"/>
+      <c r="MZ332" s="17"/>
+      <c r="NA332" s="17"/>
+      <c r="NB332" s="17"/>
+      <c r="NC332" s="17"/>
+      <c r="ND332" s="17"/>
+      <c r="NE332" s="17"/>
+      <c r="NF332" s="17"/>
+      <c r="NG332" s="17"/>
+      <c r="NH332" s="17"/>
+      <c r="NI332" s="17"/>
+      <c r="NJ332" s="17"/>
+      <c r="NK332" s="17"/>
+      <c r="NL332" s="17"/>
+      <c r="NM332" s="17"/>
+      <c r="NN332" s="17"/>
+      <c r="NO332" s="17"/>
+      <c r="NP332" s="17"/>
+      <c r="NQ332" s="17"/>
+      <c r="NR332" s="17"/>
+      <c r="NS332" s="17"/>
+      <c r="NT332" s="17"/>
+      <c r="NU332" s="17"/>
+      <c r="NV332" s="17"/>
+      <c r="NW332" s="17"/>
+      <c r="NX332" s="17"/>
+      <c r="NY332" s="17"/>
+      <c r="NZ332" s="17"/>
+      <c r="OA332" s="17"/>
+      <c r="OB332" s="17"/>
+      <c r="OC332" s="17"/>
+      <c r="OD332" s="17"/>
+      <c r="OE332" s="17"/>
+      <c r="OF332" s="17"/>
+      <c r="OG332" s="17"/>
+      <c r="OH332" s="17"/>
+      <c r="OI332" s="17"/>
+      <c r="OJ332" s="17"/>
+      <c r="OK332" s="17"/>
+      <c r="OL332" s="17"/>
+      <c r="OM332" s="17"/>
+      <c r="ON332" s="17"/>
+      <c r="OO332" s="17"/>
+      <c r="OP332" s="17"/>
+      <c r="OQ332" s="17"/>
+      <c r="OR332" s="17"/>
+      <c r="OS332" s="17"/>
+      <c r="OT332" s="17"/>
+      <c r="OU332" s="17"/>
+      <c r="OV332" s="17"/>
+      <c r="OW332" s="17"/>
+      <c r="OX332" s="17"/>
+      <c r="OY332" s="17"/>
+      <c r="OZ332" s="17"/>
+      <c r="PA332" s="17"/>
+      <c r="PB332" s="17"/>
+      <c r="PC332" s="17"/>
+      <c r="PD332" s="17"/>
+      <c r="PE332" s="17"/>
+      <c r="PF332" s="17"/>
+      <c r="PG332" s="17"/>
+      <c r="PH332" s="17"/>
+      <c r="PI332" s="17"/>
+      <c r="PJ332" s="17"/>
+      <c r="PK332" s="17"/>
+      <c r="PL332" s="17"/>
+      <c r="PM332" s="17"/>
+      <c r="PN332" s="17"/>
+      <c r="PO332" s="17"/>
+      <c r="PP332" s="17"/>
+      <c r="PQ332" s="17"/>
+      <c r="PR332" s="17"/>
+      <c r="PS332" s="17"/>
+      <c r="PT332" s="17"/>
+      <c r="PU332" s="17"/>
+      <c r="PV332" s="17"/>
+      <c r="PW332" s="17"/>
+      <c r="PX332" s="17"/>
+      <c r="PY332" s="17"/>
+      <c r="PZ332" s="17"/>
+      <c r="QA332" s="17"/>
+      <c r="QB332" s="17"/>
+      <c r="QC332" s="17"/>
+      <c r="QD332" s="17"/>
+      <c r="QE332" s="17"/>
+      <c r="QF332" s="17"/>
+    </row>
+    <row r="333" spans="1:448" s="14" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="334" spans="1:448" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A334" s="17"/>
+      <c r="B334" s="17"/>
+      <c r="C334" s="17"/>
+      <c r="D334" s="17"/>
+      <c r="E334" s="17"/>
+      <c r="F334" s="17"/>
+      <c r="G334" s="17"/>
+      <c r="H334" s="17"/>
+      <c r="I334" s="17"/>
+      <c r="J334" s="17"/>
+      <c r="K334" s="17"/>
+      <c r="L334" s="17"/>
+      <c r="M334" s="17"/>
+      <c r="N334" s="17"/>
+      <c r="O334" s="17"/>
+      <c r="P334" s="17"/>
+      <c r="Q334" s="17"/>
+      <c r="R334" s="17"/>
+      <c r="S334" s="17"/>
+      <c r="T334" s="17"/>
+      <c r="U334" s="17"/>
+      <c r="V334" s="17"/>
+      <c r="W334" s="17"/>
+      <c r="X334" s="17"/>
+      <c r="Y334" s="17"/>
+      <c r="Z334" s="17"/>
+      <c r="AA334" s="17"/>
+      <c r="AB334" s="17"/>
+      <c r="AC334" s="17"/>
+      <c r="AD334" s="17"/>
+      <c r="AE334" s="17"/>
+      <c r="AF334" s="17"/>
+      <c r="AG334" s="17"/>
+      <c r="AH334" s="17"/>
+      <c r="AI334" s="17"/>
+      <c r="AJ334" s="17"/>
+      <c r="AK334" s="17"/>
+      <c r="AL334" s="17"/>
+      <c r="AM334" s="17"/>
+      <c r="AN334" s="17"/>
+      <c r="AO334" s="17"/>
+      <c r="AP334" s="17"/>
+      <c r="AQ334" s="17"/>
+      <c r="AR334" s="17"/>
+      <c r="AS334" s="17"/>
+      <c r="AT334" s="17"/>
+      <c r="AU334" s="17"/>
+      <c r="AV334" s="17"/>
+      <c r="AW334" s="17"/>
+      <c r="AX334" s="17"/>
+      <c r="AY334" s="17"/>
+      <c r="AZ334" s="17"/>
+      <c r="BA334" s="17"/>
+      <c r="BB334" s="17"/>
+      <c r="BC334" s="17"/>
+      <c r="BD334" s="17"/>
+      <c r="BE334" s="17"/>
+      <c r="BF334" s="17"/>
+      <c r="BG334" s="17"/>
+      <c r="BH334" s="17"/>
+      <c r="BI334" s="17"/>
+      <c r="BJ334" s="17"/>
+      <c r="BK334" s="17"/>
+      <c r="BL334" s="17"/>
+      <c r="BM334" s="17"/>
+      <c r="BN334" s="17"/>
+      <c r="BO334" s="17"/>
+      <c r="BP334" s="17"/>
+      <c r="BQ334" s="17"/>
+      <c r="BR334" s="17"/>
+      <c r="BS334" s="17"/>
+      <c r="BT334" s="17"/>
+      <c r="BU334" s="17"/>
+      <c r="BV334" s="17"/>
+      <c r="BW334" s="17"/>
+      <c r="BX334" s="17"/>
+      <c r="BY334" s="17"/>
+      <c r="BZ334" s="17"/>
+      <c r="CA334" s="17"/>
+      <c r="CB334" s="17"/>
+      <c r="CC334" s="17"/>
+      <c r="CD334" s="17"/>
+      <c r="CE334" s="17"/>
+      <c r="CF334" s="17"/>
+      <c r="CG334" s="17"/>
+      <c r="CH334" s="17"/>
+      <c r="CI334" s="17"/>
+      <c r="CJ334" s="17"/>
+      <c r="CK334" s="17"/>
+      <c r="CL334" s="17"/>
+      <c r="CM334" s="17"/>
+      <c r="CN334" s="17"/>
+      <c r="CO334" s="17"/>
+      <c r="CP334" s="17"/>
+      <c r="CQ334" s="17"/>
+      <c r="CR334" s="17"/>
+      <c r="CS334" s="17"/>
+      <c r="CT334" s="17"/>
+      <c r="CU334" s="17"/>
+      <c r="CV334" s="17"/>
+      <c r="CW334" s="17"/>
+      <c r="CX334" s="17"/>
+      <c r="CY334" s="17"/>
+      <c r="CZ334" s="17"/>
+      <c r="DA334" s="17"/>
+      <c r="DB334" s="17"/>
+      <c r="DC334" s="17"/>
+      <c r="DD334" s="17"/>
+      <c r="DE334" s="17"/>
+      <c r="DF334" s="17"/>
+      <c r="DG334" s="17"/>
+      <c r="DH334" s="17"/>
+      <c r="DI334" s="17"/>
+      <c r="DJ334" s="17"/>
+      <c r="DK334" s="17"/>
+      <c r="DL334" s="17"/>
+      <c r="DM334" s="17"/>
+      <c r="DN334" s="17"/>
+      <c r="DO334" s="17"/>
+      <c r="DP334" s="17"/>
+      <c r="DQ334" s="17"/>
+      <c r="DR334" s="17"/>
+      <c r="DS334" s="17"/>
+      <c r="DT334" s="17"/>
+      <c r="DU334" s="17"/>
+      <c r="DV334" s="17"/>
+      <c r="DW334" s="17"/>
+      <c r="DX334" s="17"/>
+      <c r="DY334" s="17"/>
+      <c r="DZ334" s="17"/>
+      <c r="EA334" s="17"/>
+      <c r="EB334" s="17"/>
+      <c r="EC334" s="17"/>
+      <c r="ED334" s="17"/>
+      <c r="EE334" s="17"/>
+      <c r="EF334" s="17"/>
+      <c r="EG334" s="17"/>
+      <c r="EH334" s="17"/>
+      <c r="EI334" s="17"/>
+      <c r="EJ334" s="17"/>
+      <c r="EK334" s="17"/>
+      <c r="EL334" s="17"/>
+      <c r="EM334" s="17"/>
+      <c r="EN334" s="17"/>
+      <c r="EO334" s="17"/>
+      <c r="EP334" s="17"/>
+      <c r="EQ334" s="17"/>
+      <c r="ER334" s="17"/>
+      <c r="ES334" s="17"/>
+      <c r="ET334" s="17"/>
+      <c r="EU334" s="17"/>
+      <c r="EV334" s="17"/>
+      <c r="EW334" s="17"/>
+      <c r="EX334" s="17"/>
+      <c r="EY334" s="17"/>
+      <c r="EZ334" s="17"/>
+      <c r="FA334" s="17"/>
+      <c r="FB334" s="17"/>
+      <c r="FC334" s="17"/>
+      <c r="FD334" s="17"/>
+      <c r="FE334" s="17"/>
+      <c r="FF334" s="17"/>
+      <c r="FG334" s="17"/>
+      <c r="FH334" s="17"/>
+      <c r="FI334" s="17"/>
+      <c r="FJ334" s="17"/>
+      <c r="FK334" s="17"/>
+      <c r="FL334" s="17"/>
+      <c r="FM334" s="17"/>
+      <c r="FN334" s="17"/>
+      <c r="FO334" s="17"/>
+      <c r="FP334" s="17"/>
+      <c r="FQ334" s="17"/>
+      <c r="FR334" s="17"/>
+      <c r="FS334" s="17"/>
+      <c r="FT334" s="17"/>
+      <c r="FU334" s="17"/>
+      <c r="FV334" s="17"/>
+      <c r="FW334" s="17"/>
+      <c r="FX334" s="17"/>
+      <c r="FY334" s="17"/>
+      <c r="FZ334" s="17"/>
+      <c r="GA334" s="17"/>
+      <c r="GB334" s="17"/>
+      <c r="GC334" s="17"/>
+      <c r="GD334" s="17"/>
+      <c r="GE334" s="17"/>
+      <c r="GF334" s="17"/>
+      <c r="GG334" s="17"/>
+      <c r="GH334" s="17"/>
+      <c r="GI334" s="17"/>
+      <c r="GJ334" s="17"/>
+      <c r="GK334" s="17"/>
+      <c r="GL334" s="17"/>
+      <c r="GM334" s="17"/>
+      <c r="GN334" s="17"/>
+      <c r="GO334" s="17"/>
+      <c r="GP334" s="17"/>
+      <c r="GQ334" s="17"/>
+      <c r="GR334" s="17"/>
+      <c r="GS334" s="17"/>
+      <c r="GT334" s="17"/>
+      <c r="GU334" s="17"/>
+      <c r="GV334" s="17"/>
+      <c r="GW334" s="17"/>
+      <c r="GX334" s="17"/>
+      <c r="GY334" s="17"/>
+      <c r="GZ334" s="17"/>
+      <c r="HA334" s="17"/>
+      <c r="HB334" s="17"/>
+      <c r="HC334" s="17"/>
+      <c r="HD334" s="17"/>
+      <c r="HE334" s="17"/>
+      <c r="HF334" s="17"/>
+      <c r="HG334" s="17"/>
+      <c r="HH334" s="17"/>
+      <c r="HI334" s="17"/>
+      <c r="HJ334" s="17"/>
+      <c r="HK334" s="17"/>
+      <c r="HL334" s="17"/>
+      <c r="HM334" s="17"/>
+      <c r="HN334" s="17"/>
+      <c r="HO334" s="17"/>
+      <c r="HP334" s="17"/>
+      <c r="HQ334" s="17"/>
+      <c r="HR334" s="17"/>
+      <c r="HS334" s="17"/>
+      <c r="HT334" s="17"/>
+      <c r="HU334" s="17"/>
+      <c r="HV334" s="17"/>
+      <c r="HW334" s="17"/>
+      <c r="HX334" s="17"/>
+      <c r="HY334" s="17"/>
+      <c r="HZ334" s="17"/>
+      <c r="IA334" s="17"/>
+      <c r="IB334" s="17"/>
+      <c r="IC334" s="17"/>
+      <c r="ID334" s="17"/>
+      <c r="IE334" s="17"/>
+      <c r="IF334" s="17"/>
+      <c r="IG334" s="17"/>
+      <c r="IH334" s="17"/>
+      <c r="II334" s="17"/>
+      <c r="IJ334" s="17"/>
+      <c r="IK334" s="17"/>
+      <c r="IL334" s="17"/>
+      <c r="IM334" s="17"/>
+      <c r="IN334" s="17"/>
+      <c r="IO334" s="17"/>
+      <c r="IP334" s="17"/>
+      <c r="IQ334" s="17"/>
+      <c r="IR334" s="17"/>
+      <c r="IS334" s="17"/>
+      <c r="IT334" s="17"/>
+      <c r="IU334" s="17"/>
+      <c r="IV334" s="17"/>
+      <c r="IW334" s="17"/>
+      <c r="IX334" s="17"/>
+      <c r="IY334" s="17"/>
+      <c r="IZ334" s="17"/>
+      <c r="JA334" s="17"/>
+      <c r="JB334" s="17"/>
+      <c r="JC334" s="17"/>
+      <c r="JD334" s="17"/>
+      <c r="JE334" s="17"/>
+      <c r="JF334" s="17"/>
+      <c r="JG334" s="17"/>
+      <c r="JH334" s="17"/>
+      <c r="JI334" s="17"/>
+      <c r="JJ334" s="17"/>
+      <c r="JK334" s="17"/>
+      <c r="JL334" s="17"/>
+      <c r="JM334" s="17"/>
+      <c r="JN334" s="17"/>
+      <c r="JO334" s="17"/>
+      <c r="JP334" s="17"/>
+      <c r="JQ334" s="17"/>
+      <c r="JR334" s="17"/>
+      <c r="JS334" s="17"/>
+      <c r="JT334" s="17"/>
+      <c r="JU334" s="17"/>
+      <c r="JV334" s="17"/>
+      <c r="JW334" s="17"/>
+      <c r="JX334" s="17"/>
+      <c r="JY334" s="17"/>
+      <c r="JZ334" s="17"/>
+      <c r="KA334" s="17"/>
+      <c r="KB334" s="17"/>
+      <c r="KC334" s="17"/>
+      <c r="KD334" s="17"/>
+      <c r="KE334" s="17"/>
+      <c r="KF334" s="17"/>
+      <c r="KG334" s="17"/>
+      <c r="KH334" s="17"/>
+      <c r="KI334" s="17"/>
+      <c r="KJ334" s="17"/>
+      <c r="KK334" s="17"/>
+      <c r="KL334" s="17"/>
+      <c r="KM334" s="17"/>
+      <c r="KN334" s="17"/>
+      <c r="KO334" s="17"/>
+      <c r="KP334" s="17"/>
+      <c r="KQ334" s="17"/>
+      <c r="KR334" s="17"/>
+      <c r="KS334" s="17"/>
+      <c r="KT334" s="17"/>
+      <c r="KU334" s="17"/>
+      <c r="KV334" s="17"/>
+      <c r="KW334" s="17"/>
+      <c r="KX334" s="17"/>
+      <c r="KY334" s="17"/>
+      <c r="KZ334" s="17"/>
+      <c r="LA334" s="17"/>
+      <c r="LB334" s="17"/>
+      <c r="LC334" s="17"/>
+      <c r="LD334" s="17"/>
+      <c r="LE334" s="17"/>
+      <c r="LF334" s="17"/>
+      <c r="LG334" s="17"/>
+      <c r="LH334" s="17"/>
+      <c r="LI334" s="17"/>
+      <c r="LJ334" s="17"/>
+      <c r="LK334" s="17"/>
+      <c r="LL334" s="17"/>
+      <c r="LM334" s="17"/>
+      <c r="LN334" s="17"/>
+      <c r="LO334" s="17"/>
+      <c r="LP334" s="17"/>
+      <c r="LQ334" s="17"/>
+      <c r="LR334" s="17"/>
+      <c r="LS334" s="17"/>
+      <c r="LT334" s="17"/>
+      <c r="LU334" s="17"/>
+      <c r="LV334" s="17"/>
+      <c r="LW334" s="17"/>
+      <c r="LX334" s="17"/>
+      <c r="LY334" s="17"/>
+      <c r="LZ334" s="17"/>
+      <c r="MA334" s="17"/>
+      <c r="MB334" s="17"/>
+      <c r="MC334" s="17"/>
+      <c r="MD334" s="17"/>
+      <c r="ME334" s="17"/>
+      <c r="MF334" s="17"/>
+      <c r="MG334" s="17"/>
+      <c r="MH334" s="17"/>
+      <c r="MI334" s="17"/>
+      <c r="MJ334" s="17"/>
+      <c r="MK334" s="17"/>
+      <c r="ML334" s="17"/>
+      <c r="MM334" s="17"/>
+      <c r="MN334" s="17"/>
+      <c r="MO334" s="17"/>
+      <c r="MP334" s="17"/>
+      <c r="MQ334" s="17"/>
+      <c r="MR334" s="17"/>
+      <c r="MS334" s="17"/>
+      <c r="MT334" s="17"/>
+      <c r="MU334" s="17"/>
+      <c r="MV334" s="17"/>
+      <c r="MW334" s="17"/>
+      <c r="MX334" s="17"/>
+      <c r="MY334" s="17"/>
+      <c r="MZ334" s="17"/>
+      <c r="NA334" s="17"/>
+      <c r="NB334" s="17"/>
+      <c r="NC334" s="17"/>
+      <c r="ND334" s="17"/>
+      <c r="NE334" s="17"/>
+      <c r="NF334" s="17"/>
+      <c r="NG334" s="17"/>
+      <c r="NH334" s="17"/>
+      <c r="NI334" s="17"/>
+      <c r="NJ334" s="17"/>
+      <c r="NK334" s="17"/>
+      <c r="NL334" s="17"/>
+      <c r="NM334" s="17"/>
+      <c r="NN334" s="17"/>
+      <c r="NO334" s="17"/>
+      <c r="NP334" s="17"/>
+      <c r="NQ334" s="17"/>
+      <c r="NR334" s="17"/>
+      <c r="NS334" s="17"/>
+      <c r="NT334" s="17"/>
+      <c r="NU334" s="17"/>
+      <c r="NV334" s="17"/>
+      <c r="NW334" s="17"/>
+      <c r="NX334" s="17"/>
+      <c r="NY334" s="17"/>
+      <c r="NZ334" s="17"/>
+      <c r="OA334" s="17"/>
+      <c r="OB334" s="17"/>
+      <c r="OC334" s="17"/>
+      <c r="OD334" s="17"/>
+      <c r="OE334" s="17"/>
+      <c r="OF334" s="17"/>
+      <c r="OG334" s="17"/>
+      <c r="OH334" s="17"/>
+      <c r="OI334" s="17"/>
+      <c r="OJ334" s="17"/>
+      <c r="OK334" s="17"/>
+      <c r="OL334" s="17"/>
+      <c r="OM334" s="17"/>
+      <c r="ON334" s="17"/>
+      <c r="OO334" s="17"/>
+      <c r="OP334" s="17"/>
+      <c r="OQ334" s="17"/>
+      <c r="OR334" s="17"/>
+      <c r="OS334" s="17"/>
+      <c r="OT334" s="17"/>
+      <c r="OU334" s="17"/>
+      <c r="OV334" s="17"/>
+      <c r="OW334" s="17"/>
+      <c r="OX334" s="17"/>
+      <c r="OY334" s="17"/>
+      <c r="OZ334" s="17"/>
+      <c r="PA334" s="17"/>
+      <c r="PB334" s="17"/>
+      <c r="PC334" s="17"/>
+      <c r="PD334" s="17"/>
+      <c r="PE334" s="17"/>
+      <c r="PF334" s="17"/>
+      <c r="PG334" s="17"/>
+      <c r="PH334" s="17"/>
+      <c r="PI334" s="17"/>
+      <c r="PJ334" s="17"/>
+      <c r="PK334" s="17"/>
+      <c r="PL334" s="17"/>
+      <c r="PM334" s="17"/>
+      <c r="PN334" s="17"/>
+      <c r="PO334" s="17"/>
+      <c r="PP334" s="17"/>
+      <c r="PQ334" s="17"/>
+      <c r="PR334" s="17"/>
+      <c r="PS334" s="17"/>
+      <c r="PT334" s="17"/>
+      <c r="PU334" s="17"/>
+      <c r="PV334" s="17"/>
+      <c r="PW334" s="17"/>
+      <c r="PX334" s="17"/>
+      <c r="PY334" s="17"/>
+      <c r="PZ334" s="17"/>
+      <c r="QA334" s="17"/>
+      <c r="QB334" s="17"/>
+      <c r="QC334" s="17"/>
+      <c r="QD334" s="17"/>
+      <c r="QE334" s="17"/>
+      <c r="QF334" s="17"/>
+    </row>
+    <row r="335" spans="1:448" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="336" spans="1:448" s="23" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A336" s="23" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="329" spans="1:448" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="330" spans="1:448" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A330" s="14" t="s">
-        <v>363</v>
-      </c>
-      <c r="D330" s="14" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="331" spans="1:448" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A331" s="17"/>
-      <c r="B331" s="17"/>
-      <c r="C331" s="17"/>
-      <c r="D331" s="17"/>
-      <c r="E331" s="17"/>
-      <c r="F331" s="17"/>
-      <c r="G331" s="17"/>
-      <c r="H331" s="17"/>
-      <c r="I331" s="17"/>
-      <c r="J331" s="17"/>
-      <c r="K331" s="17"/>
-      <c r="L331" s="17"/>
-      <c r="M331" s="17"/>
-      <c r="N331" s="17"/>
-      <c r="O331" s="17"/>
-      <c r="P331" s="17"/>
-      <c r="Q331" s="17"/>
-      <c r="R331" s="17"/>
-      <c r="S331" s="17"/>
-      <c r="T331" s="17"/>
-      <c r="U331" s="17"/>
-      <c r="V331" s="17"/>
-      <c r="W331" s="17"/>
-      <c r="X331" s="17"/>
-      <c r="Y331" s="17"/>
-      <c r="Z331" s="17"/>
-      <c r="AA331" s="17"/>
-      <c r="AB331" s="17"/>
-      <c r="AC331" s="17"/>
-      <c r="AD331" s="17"/>
-      <c r="AE331" s="17"/>
-      <c r="AF331" s="17"/>
-      <c r="AG331" s="17"/>
-      <c r="AH331" s="17"/>
-      <c r="AI331" s="17"/>
-      <c r="AJ331" s="17"/>
-      <c r="AK331" s="17"/>
-      <c r="AL331" s="17"/>
-      <c r="AM331" s="17"/>
-      <c r="AN331" s="17"/>
-      <c r="AO331" s="17"/>
-      <c r="AP331" s="17"/>
-      <c r="AQ331" s="17"/>
-      <c r="AR331" s="17"/>
-      <c r="AS331" s="17"/>
-      <c r="AT331" s="17"/>
-      <c r="AU331" s="17"/>
-      <c r="AV331" s="17"/>
-      <c r="AW331" s="17"/>
-      <c r="AX331" s="17"/>
-      <c r="AY331" s="17"/>
-      <c r="AZ331" s="17"/>
-      <c r="BA331" s="17"/>
-      <c r="BB331" s="17"/>
-      <c r="BC331" s="17"/>
-      <c r="BD331" s="17"/>
-      <c r="BE331" s="17"/>
-      <c r="BF331" s="17"/>
-      <c r="BG331" s="17"/>
-      <c r="BH331" s="17"/>
-      <c r="BI331" s="17"/>
-      <c r="BJ331" s="17"/>
-      <c r="BK331" s="17"/>
-      <c r="BL331" s="17"/>
-      <c r="BM331" s="17"/>
-      <c r="BN331" s="17"/>
-      <c r="BO331" s="17"/>
-      <c r="BP331" s="17"/>
-      <c r="BQ331" s="17"/>
-      <c r="BR331" s="17"/>
-      <c r="BS331" s="17"/>
-      <c r="BT331" s="17"/>
-      <c r="BU331" s="17"/>
-      <c r="BV331" s="17"/>
-    </row>
-    <row r="332" spans="1:448" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A332" s="14" t="s">
-        <v>364</v>
-      </c>
-      <c r="D332" s="14" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="333" spans="1:448" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A333" s="17"/>
-      <c r="B333" s="17"/>
-      <c r="C333" s="17"/>
-      <c r="D333" s="17"/>
-      <c r="E333" s="17"/>
-      <c r="F333" s="17"/>
-      <c r="G333" s="17"/>
-      <c r="H333" s="17"/>
-      <c r="I333" s="17"/>
-      <c r="J333" s="17"/>
-      <c r="K333" s="17"/>
-      <c r="L333" s="17"/>
-      <c r="M333" s="17"/>
-      <c r="N333" s="17"/>
-      <c r="O333" s="17"/>
-      <c r="P333" s="17"/>
-      <c r="Q333" s="17"/>
-      <c r="R333" s="17"/>
-      <c r="S333" s="17"/>
-      <c r="T333" s="17"/>
-      <c r="U333" s="17"/>
-      <c r="V333" s="17"/>
-      <c r="W333" s="17"/>
-      <c r="X333" s="17"/>
-      <c r="Y333" s="17"/>
-      <c r="Z333" s="17"/>
-      <c r="AA333" s="17"/>
-      <c r="AB333" s="17"/>
-      <c r="AC333" s="17"/>
-      <c r="AD333" s="17"/>
-      <c r="AE333" s="17"/>
-      <c r="AF333" s="17"/>
-      <c r="AG333" s="17"/>
-      <c r="AH333" s="17"/>
-      <c r="AI333" s="17"/>
-      <c r="AJ333" s="17"/>
-      <c r="AK333" s="17"/>
-      <c r="AL333" s="17"/>
-      <c r="AM333" s="17"/>
-      <c r="AN333" s="17"/>
-      <c r="AO333" s="17"/>
-      <c r="AP333" s="17"/>
-      <c r="AQ333" s="17"/>
-      <c r="AR333" s="17"/>
-      <c r="AS333" s="17"/>
-      <c r="AT333" s="17"/>
-      <c r="AU333" s="17"/>
-      <c r="AV333" s="17"/>
-      <c r="AW333" s="17"/>
-      <c r="AX333" s="17"/>
-      <c r="AY333" s="17"/>
-      <c r="AZ333" s="17"/>
-      <c r="BA333" s="17"/>
-      <c r="BB333" s="17"/>
-      <c r="BC333" s="17"/>
-      <c r="BD333" s="17"/>
-      <c r="BE333" s="17"/>
-      <c r="BF333" s="17"/>
-      <c r="BG333" s="17"/>
-      <c r="BH333" s="17"/>
-      <c r="BI333" s="17"/>
-      <c r="BJ333" s="17"/>
-      <c r="BK333" s="17"/>
-      <c r="BL333" s="17"/>
-      <c r="BM333" s="17"/>
-      <c r="BN333" s="17"/>
-      <c r="BO333" s="17"/>
-      <c r="BP333" s="17"/>
-      <c r="BQ333" s="17"/>
-      <c r="BR333" s="17"/>
-      <c r="BS333" s="17"/>
-      <c r="BT333" s="17"/>
-      <c r="BU333" s="17"/>
-      <c r="BV333" s="17"/>
-    </row>
-    <row r="334" spans="1:448" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A334" s="14" t="s">
-        <v>365</v>
-      </c>
-      <c r="D334" s="14" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="335" spans="1:448" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A335" s="17"/>
-      <c r="B335" s="17"/>
-      <c r="C335" s="17"/>
-      <c r="D335" s="17"/>
-      <c r="E335" s="17"/>
-      <c r="F335" s="17"/>
-      <c r="G335" s="17"/>
-      <c r="H335" s="17"/>
-      <c r="I335" s="17"/>
-      <c r="J335" s="17"/>
-      <c r="K335" s="17"/>
-      <c r="L335" s="17"/>
-      <c r="M335" s="17"/>
-      <c r="N335" s="17"/>
-      <c r="O335" s="17"/>
-      <c r="P335" s="17"/>
-      <c r="Q335" s="17"/>
-      <c r="R335" s="17"/>
-      <c r="S335" s="17"/>
-      <c r="T335" s="17"/>
-      <c r="U335" s="17"/>
-      <c r="V335" s="17"/>
-      <c r="W335" s="17"/>
-      <c r="X335" s="17"/>
-      <c r="Y335" s="17"/>
-      <c r="Z335" s="17"/>
-      <c r="AA335" s="17"/>
-      <c r="AB335" s="17"/>
-      <c r="AC335" s="17"/>
-      <c r="AD335" s="17"/>
-      <c r="AE335" s="17"/>
-      <c r="AF335" s="17"/>
-      <c r="AG335" s="17"/>
-      <c r="AH335" s="17"/>
-      <c r="AI335" s="17"/>
-      <c r="AJ335" s="17"/>
-      <c r="AK335" s="17"/>
-      <c r="AL335" s="17"/>
-      <c r="AM335" s="17"/>
-      <c r="AN335" s="17"/>
-      <c r="AO335" s="17"/>
-      <c r="AP335" s="17"/>
-      <c r="AQ335" s="17"/>
-      <c r="AR335" s="17"/>
-      <c r="AS335" s="17"/>
-      <c r="AT335" s="17"/>
-      <c r="AU335" s="17"/>
-      <c r="AV335" s="17"/>
-      <c r="AW335" s="17"/>
-      <c r="AX335" s="17"/>
-      <c r="AY335" s="17"/>
-      <c r="AZ335" s="17"/>
-      <c r="BA335" s="17"/>
-      <c r="BB335" s="17"/>
-      <c r="BC335" s="17"/>
-      <c r="BD335" s="17"/>
-      <c r="BE335" s="17"/>
-      <c r="BF335" s="17"/>
-      <c r="BG335" s="17"/>
-      <c r="BH335" s="17"/>
-      <c r="BI335" s="17"/>
-      <c r="BJ335" s="17"/>
-      <c r="BK335" s="17"/>
-      <c r="BL335" s="17"/>
-      <c r="BM335" s="17"/>
-      <c r="BN335" s="17"/>
-      <c r="BO335" s="17"/>
-      <c r="BP335" s="17"/>
-      <c r="BQ335" s="17"/>
-      <c r="BR335" s="17"/>
-      <c r="BS335" s="17"/>
-      <c r="BT335" s="17"/>
-      <c r="BU335" s="17"/>
-      <c r="BV335" s="17"/>
-    </row>
-    <row r="336" spans="1:448" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A336" s="14" t="s">
-        <v>366</v>
-      </c>
-      <c r="D336" s="14" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="337" spans="1:74" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A337" s="17"/>
-      <c r="B337" s="17"/>
-      <c r="C337" s="17"/>
-      <c r="D337" s="17"/>
-      <c r="E337" s="17"/>
-      <c r="F337" s="17"/>
-      <c r="G337" s="17"/>
-      <c r="H337" s="17"/>
-      <c r="I337" s="17"/>
-      <c r="J337" s="17"/>
-      <c r="K337" s="17"/>
-      <c r="L337" s="17"/>
-      <c r="M337" s="17"/>
-      <c r="N337" s="17"/>
-      <c r="O337" s="17"/>
-      <c r="P337" s="17"/>
-      <c r="Q337" s="17"/>
-      <c r="R337" s="17"/>
-      <c r="S337" s="17"/>
-      <c r="T337" s="17"/>
-      <c r="U337" s="17"/>
-      <c r="V337" s="17"/>
-      <c r="W337" s="17"/>
-      <c r="X337" s="17"/>
-      <c r="Y337" s="17"/>
-      <c r="Z337" s="17"/>
-      <c r="AA337" s="17"/>
-      <c r="AB337" s="17"/>
-      <c r="AC337" s="17"/>
-      <c r="AD337" s="17"/>
-      <c r="AE337" s="17"/>
-      <c r="AF337" s="17"/>
-      <c r="AG337" s="17"/>
-      <c r="AH337" s="17"/>
-      <c r="AI337" s="17"/>
-      <c r="AJ337" s="17"/>
-      <c r="AK337" s="17"/>
-      <c r="AL337" s="17"/>
-      <c r="AM337" s="17"/>
-      <c r="AN337" s="17"/>
-      <c r="AO337" s="17"/>
-      <c r="AP337" s="17"/>
-      <c r="AQ337" s="17"/>
-      <c r="AR337" s="17"/>
-      <c r="AS337" s="17"/>
-      <c r="AT337" s="17"/>
-      <c r="AU337" s="17"/>
-      <c r="AV337" s="17"/>
-      <c r="AW337" s="17"/>
-      <c r="AX337" s="17"/>
-      <c r="AY337" s="17"/>
-      <c r="AZ337" s="17"/>
-      <c r="BA337" s="17"/>
-      <c r="BB337" s="17"/>
-      <c r="BC337" s="17"/>
-      <c r="BD337" s="17"/>
-      <c r="BE337" s="17"/>
-      <c r="BF337" s="17"/>
-      <c r="BG337" s="17"/>
-      <c r="BH337" s="17"/>
-      <c r="BI337" s="17"/>
-      <c r="BJ337" s="17"/>
-      <c r="BK337" s="17"/>
-      <c r="BL337" s="17"/>
-      <c r="BM337" s="17"/>
-      <c r="BN337" s="17"/>
-      <c r="BO337" s="17"/>
-      <c r="BP337" s="17"/>
-      <c r="BQ337" s="17"/>
-      <c r="BR337" s="17"/>
-      <c r="BS337" s="17"/>
-      <c r="BT337" s="17"/>
-      <c r="BU337" s="17"/>
-      <c r="BV337" s="17"/>
-    </row>
+    <row r="337" spans="1:74" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="338" spans="1:74" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A338" s="14" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="D338" s="14" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
     </row>
     <row r="339" spans="1:74" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -8812,10 +10307,10 @@
     </row>
     <row r="340" spans="1:74" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A340" s="14" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="D340" s="14" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
     </row>
     <row r="341" spans="1:74" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -8896,10 +10391,10 @@
     </row>
     <row r="342" spans="1:74" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A342" s="14" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="D342" s="14" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
     </row>
     <row r="343" spans="1:74" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -8980,10 +10475,10 @@
     </row>
     <row r="344" spans="1:74" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A344" s="14" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="D344" s="14" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
     </row>
     <row r="345" spans="1:74" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -9064,10 +10559,10 @@
     </row>
     <row r="346" spans="1:74" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A346" s="14" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="D346" s="14" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
     </row>
     <row r="347" spans="1:74" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -9146,12 +10641,12 @@
       <c r="BU347" s="17"/>
       <c r="BV347" s="17"/>
     </row>
-    <row r="348" spans="1:74" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A348" s="9" t="s">
-        <v>372</v>
-      </c>
-      <c r="D348" s="9" t="s">
-        <v>408</v>
+    <row r="348" spans="1:74" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A348" s="14" t="s">
+        <v>368</v>
+      </c>
+      <c r="D348" s="14" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="349" spans="1:74" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -9230,12 +10725,12 @@
       <c r="BU349" s="17"/>
       <c r="BV349" s="17"/>
     </row>
-    <row r="350" spans="1:74" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A350" s="9" t="s">
-        <v>373</v>
-      </c>
-      <c r="D350" s="9" t="s">
-        <v>409</v>
+    <row r="350" spans="1:74" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A350" s="14" t="s">
+        <v>369</v>
+      </c>
+      <c r="D350" s="14" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="351" spans="1:74" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -9314,15 +10809,12 @@
       <c r="BU351" s="17"/>
       <c r="BV351" s="17"/>
     </row>
-    <row r="352" spans="1:74" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A352" s="9" t="s">
-        <v>374</v>
-      </c>
-      <c r="B352" s="9" t="s">
-        <v>303</v>
-      </c>
-      <c r="D352" s="9" t="s">
-        <v>410</v>
+    <row r="352" spans="1:74" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A352" s="14" t="s">
+        <v>370</v>
+      </c>
+      <c r="D352" s="14" t="s">
+        <v>406</v>
       </c>
     </row>
     <row r="353" spans="1:74" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -9401,12 +10893,12 @@
       <c r="BU353" s="17"/>
       <c r="BV353" s="17"/>
     </row>
-    <row r="354" spans="1:74" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A354" s="9" t="s">
-        <v>375</v>
-      </c>
-      <c r="D354" s="9" t="s">
-        <v>411</v>
+    <row r="354" spans="1:74" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A354" s="14" t="s">
+        <v>371</v>
+      </c>
+      <c r="D354" s="14" t="s">
+        <v>407</v>
       </c>
     </row>
     <row r="355" spans="1:74" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -9487,10 +10979,10 @@
     </row>
     <row r="356" spans="1:74" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A356" s="9" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="D356" s="9" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
     </row>
     <row r="357" spans="1:74" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -9571,10 +11063,10 @@
     </row>
     <row r="358" spans="1:74" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A358" s="9" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="D358" s="9" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
     </row>
     <row r="359" spans="1:74" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -9655,10 +11147,13 @@
     </row>
     <row r="360" spans="1:74" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A360" s="9" t="s">
-        <v>345</v>
+        <v>374</v>
+      </c>
+      <c r="B360" s="9" t="s">
+        <v>303</v>
       </c>
       <c r="D360" s="9" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
     </row>
     <row r="361" spans="1:74" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -9739,10 +11234,10 @@
     </row>
     <row r="362" spans="1:74" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A362" s="9" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="D362" s="9" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
     </row>
     <row r="363" spans="1:74" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -9823,10 +11318,10 @@
     </row>
     <row r="364" spans="1:74" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A364" s="9" t="s">
-        <v>419</v>
+        <v>376</v>
       </c>
       <c r="D364" s="9" t="s">
-        <v>420</v>
+        <v>412</v>
       </c>
     </row>
     <row r="365" spans="1:74" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -9907,10 +11402,10 @@
     </row>
     <row r="366" spans="1:74" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A366" s="9" t="s">
-        <v>421</v>
+        <v>377</v>
       </c>
       <c r="D366" s="9" t="s">
-        <v>422</v>
+        <v>413</v>
       </c>
     </row>
     <row r="367" spans="1:74" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -9991,10 +11486,10 @@
     </row>
     <row r="368" spans="1:74" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A368" s="9" t="s">
-        <v>423</v>
+        <v>345</v>
       </c>
       <c r="D368" s="9" t="s">
-        <v>424</v>
+        <v>414</v>
       </c>
     </row>
     <row r="369" spans="1:74" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -10073,7 +11568,14 @@
       <c r="BU369" s="17"/>
       <c r="BV369" s="17"/>
     </row>
-    <row r="370" spans="1:74" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="370" spans="1:74" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A370" s="9" t="s">
+        <v>378</v>
+      </c>
+      <c r="D370" s="9" t="s">
+        <v>415</v>
+      </c>
+    </row>
     <row r="371" spans="1:74" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A371" s="17"/>
       <c r="B371" s="17"/>
@@ -10150,7 +11652,14 @@
       <c r="BU371" s="17"/>
       <c r="BV371" s="17"/>
     </row>
-    <row r="372" spans="1:74" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="372" spans="1:74" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A372" s="9" t="s">
+        <v>419</v>
+      </c>
+      <c r="D372" s="9" t="s">
+        <v>420</v>
+      </c>
+    </row>
     <row r="373" spans="1:74" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A373" s="17"/>
       <c r="B373" s="17"/>
@@ -10227,7 +11736,14 @@
       <c r="BU373" s="17"/>
       <c r="BV373" s="17"/>
     </row>
-    <row r="374" spans="1:74" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="374" spans="1:74" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A374" s="9" t="s">
+        <v>421</v>
+      </c>
+      <c r="D374" s="9" t="s">
+        <v>422</v>
+      </c>
+    </row>
     <row r="375" spans="1:74" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A375" s="17"/>
       <c r="B375" s="17"/>
@@ -10304,6 +11820,14 @@
       <c r="BU375" s="17"/>
       <c r="BV375" s="17"/>
     </row>
+    <row r="376" spans="1:74" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A376" s="9" t="s">
+        <v>423</v>
+      </c>
+      <c r="D376" s="9" t="s">
+        <v>424</v>
+      </c>
+    </row>
     <row r="377" spans="1:74" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A377" s="17"/>
       <c r="B377" s="17"/>
@@ -10380,6 +11904,11 @@
       <c r="BU377" s="17"/>
       <c r="BV377" s="17"/>
     </row>
+    <row r="378" spans="1:74" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A378" s="9" t="s">
+        <v>425</v>
+      </c>
+    </row>
     <row r="379" spans="1:74" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A379" s="17"/>
       <c r="B379" s="17"/>
@@ -10456,6 +11985,11 @@
       <c r="BU379" s="17"/>
       <c r="BV379" s="17"/>
     </row>
+    <row r="380" spans="1:74" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A380" s="9" t="s">
+        <v>426</v>
+      </c>
+    </row>
     <row r="381" spans="1:74" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A381" s="17"/>
       <c r="B381" s="17"/>
@@ -10532,6 +12066,7 @@
       <c r="BU381" s="17"/>
       <c r="BV381" s="17"/>
     </row>
+    <row r="382" spans="1:74" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="383" spans="1:74" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A383" s="17"/>
       <c r="B383" s="17"/>
@@ -10608,129 +12143,321 @@
       <c r="BU383" s="17"/>
       <c r="BV383" s="17"/>
     </row>
-    <row r="428" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A428" s="12"/>
-      <c r="B428" s="12"/>
-      <c r="C428" s="12"/>
-      <c r="D428" s="12"/>
-      <c r="E428" s="12"/>
-      <c r="F428" s="12"/>
-      <c r="G428" s="12"/>
-      <c r="H428" s="12"/>
-      <c r="I428" s="12"/>
-      <c r="J428" s="12"/>
-      <c r="K428" s="12"/>
-      <c r="L428" s="12"/>
-    </row>
-    <row r="429" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A429" s="12"/>
-      <c r="B429" s="12"/>
-      <c r="C429" s="12"/>
-      <c r="D429" s="12"/>
-      <c r="E429" s="12"/>
-      <c r="F429" s="12"/>
-      <c r="G429" s="12"/>
-      <c r="H429" s="12"/>
-      <c r="I429" s="12"/>
-      <c r="J429" s="12"/>
-      <c r="K429" s="12"/>
-      <c r="L429" s="12"/>
-    </row>
-    <row r="430" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A430" s="12"/>
-      <c r="B430" s="12"/>
-      <c r="C430" s="12"/>
-      <c r="D430" s="12"/>
-      <c r="E430" s="12"/>
-      <c r="F430" s="12"/>
-      <c r="G430" s="12"/>
-      <c r="H430" s="12"/>
-      <c r="I430" s="12"/>
-      <c r="J430" s="12"/>
-      <c r="K430" s="12"/>
-      <c r="L430" s="12"/>
-    </row>
-    <row r="431" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A431" s="12"/>
-      <c r="B431" s="12"/>
-      <c r="C431" s="12"/>
-      <c r="D431" s="12"/>
-      <c r="E431" s="12"/>
-      <c r="F431" s="12"/>
-      <c r="G431" s="12"/>
-      <c r="H431" s="12"/>
-      <c r="I431" s="12"/>
-      <c r="J431" s="12"/>
-      <c r="K431" s="12"/>
-      <c r="L431" s="12"/>
-    </row>
-    <row r="432" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A432" s="14"/>
-      <c r="B432" s="14"/>
-      <c r="C432" s="14"/>
-      <c r="D432" s="14"/>
-      <c r="E432" s="14"/>
-      <c r="F432" s="14"/>
-      <c r="G432" s="14"/>
-      <c r="H432" s="14"/>
-      <c r="I432" s="14"/>
-      <c r="J432" s="14"/>
-      <c r="K432" s="12"/>
-      <c r="L432" s="12"/>
-    </row>
-    <row r="433" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A433" s="14"/>
-      <c r="B433" s="14"/>
-      <c r="C433" s="14"/>
-      <c r="D433" s="14"/>
-      <c r="E433" s="14"/>
-      <c r="F433" s="14"/>
-      <c r="G433" s="14"/>
-      <c r="H433" s="14"/>
-      <c r="I433" s="14"/>
-      <c r="J433" s="14"/>
-      <c r="K433" s="12"/>
-      <c r="L433" s="12"/>
-    </row>
-    <row r="434" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A434" s="14"/>
-      <c r="B434" s="14"/>
-      <c r="C434" s="14"/>
-      <c r="D434" s="14"/>
-      <c r="E434" s="14"/>
-      <c r="F434" s="14"/>
-      <c r="G434" s="14"/>
-      <c r="H434" s="14"/>
-      <c r="I434" s="14"/>
-      <c r="J434" s="14"/>
-      <c r="K434" s="12"/>
-      <c r="L434" s="12"/>
-    </row>
-    <row r="435" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A435" s="14"/>
-      <c r="B435" s="14"/>
-      <c r="C435" s="14"/>
-      <c r="D435" s="14"/>
-      <c r="E435" s="14"/>
-      <c r="F435" s="14"/>
-      <c r="G435" s="14"/>
-      <c r="H435" s="14"/>
-      <c r="I435" s="14"/>
-      <c r="J435" s="14"/>
-      <c r="K435" s="12"/>
-      <c r="L435" s="12"/>
-    </row>
-    <row r="436" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A436" s="14"/>
-      <c r="B436" s="14"/>
-      <c r="C436" s="14"/>
-      <c r="D436" s="14"/>
-      <c r="E436" s="14"/>
-      <c r="F436" s="14"/>
-      <c r="G436" s="14"/>
-      <c r="H436" s="14"/>
-      <c r="I436" s="14"/>
-      <c r="J436" s="14"/>
+    <row r="385" spans="1:74" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A385" s="17"/>
+      <c r="B385" s="17"/>
+      <c r="C385" s="17"/>
+      <c r="D385" s="17"/>
+      <c r="E385" s="17"/>
+      <c r="F385" s="17"/>
+      <c r="G385" s="17"/>
+      <c r="H385" s="17"/>
+      <c r="I385" s="17"/>
+      <c r="J385" s="17"/>
+      <c r="K385" s="17"/>
+      <c r="L385" s="17"/>
+      <c r="M385" s="17"/>
+      <c r="N385" s="17"/>
+      <c r="O385" s="17"/>
+      <c r="P385" s="17"/>
+      <c r="Q385" s="17"/>
+      <c r="R385" s="17"/>
+      <c r="S385" s="17"/>
+      <c r="T385" s="17"/>
+      <c r="U385" s="17"/>
+      <c r="V385" s="17"/>
+      <c r="W385" s="17"/>
+      <c r="X385" s="17"/>
+      <c r="Y385" s="17"/>
+      <c r="Z385" s="17"/>
+      <c r="AA385" s="17"/>
+      <c r="AB385" s="17"/>
+      <c r="AC385" s="17"/>
+      <c r="AD385" s="17"/>
+      <c r="AE385" s="17"/>
+      <c r="AF385" s="17"/>
+      <c r="AG385" s="17"/>
+      <c r="AH385" s="17"/>
+      <c r="AI385" s="17"/>
+      <c r="AJ385" s="17"/>
+      <c r="AK385" s="17"/>
+      <c r="AL385" s="17"/>
+      <c r="AM385" s="17"/>
+      <c r="AN385" s="17"/>
+      <c r="AO385" s="17"/>
+      <c r="AP385" s="17"/>
+      <c r="AQ385" s="17"/>
+      <c r="AR385" s="17"/>
+      <c r="AS385" s="17"/>
+      <c r="AT385" s="17"/>
+      <c r="AU385" s="17"/>
+      <c r="AV385" s="17"/>
+      <c r="AW385" s="17"/>
+      <c r="AX385" s="17"/>
+      <c r="AY385" s="17"/>
+      <c r="AZ385" s="17"/>
+      <c r="BA385" s="17"/>
+      <c r="BB385" s="17"/>
+      <c r="BC385" s="17"/>
+      <c r="BD385" s="17"/>
+      <c r="BE385" s="17"/>
+      <c r="BF385" s="17"/>
+      <c r="BG385" s="17"/>
+      <c r="BH385" s="17"/>
+      <c r="BI385" s="17"/>
+      <c r="BJ385" s="17"/>
+      <c r="BK385" s="17"/>
+      <c r="BL385" s="17"/>
+      <c r="BM385" s="17"/>
+      <c r="BN385" s="17"/>
+      <c r="BO385" s="17"/>
+      <c r="BP385" s="17"/>
+      <c r="BQ385" s="17"/>
+      <c r="BR385" s="17"/>
+      <c r="BS385" s="17"/>
+      <c r="BT385" s="17"/>
+      <c r="BU385" s="17"/>
+      <c r="BV385" s="17"/>
+    </row>
+    <row r="387" spans="1:74" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A387" s="17"/>
+      <c r="B387" s="17"/>
+      <c r="C387" s="17"/>
+      <c r="D387" s="17"/>
+      <c r="E387" s="17"/>
+      <c r="F387" s="17"/>
+      <c r="G387" s="17"/>
+      <c r="H387" s="17"/>
+      <c r="I387" s="17"/>
+      <c r="J387" s="17"/>
+      <c r="K387" s="17"/>
+      <c r="L387" s="17"/>
+      <c r="M387" s="17"/>
+      <c r="N387" s="17"/>
+      <c r="O387" s="17"/>
+      <c r="P387" s="17"/>
+      <c r="Q387" s="17"/>
+      <c r="R387" s="17"/>
+      <c r="S387" s="17"/>
+      <c r="T387" s="17"/>
+      <c r="U387" s="17"/>
+      <c r="V387" s="17"/>
+      <c r="W387" s="17"/>
+      <c r="X387" s="17"/>
+      <c r="Y387" s="17"/>
+      <c r="Z387" s="17"/>
+      <c r="AA387" s="17"/>
+      <c r="AB387" s="17"/>
+      <c r="AC387" s="17"/>
+      <c r="AD387" s="17"/>
+      <c r="AE387" s="17"/>
+      <c r="AF387" s="17"/>
+      <c r="AG387" s="17"/>
+      <c r="AH387" s="17"/>
+      <c r="AI387" s="17"/>
+      <c r="AJ387" s="17"/>
+      <c r="AK387" s="17"/>
+      <c r="AL387" s="17"/>
+      <c r="AM387" s="17"/>
+      <c r="AN387" s="17"/>
+      <c r="AO387" s="17"/>
+      <c r="AP387" s="17"/>
+      <c r="AQ387" s="17"/>
+      <c r="AR387" s="17"/>
+      <c r="AS387" s="17"/>
+      <c r="AT387" s="17"/>
+      <c r="AU387" s="17"/>
+      <c r="AV387" s="17"/>
+      <c r="AW387" s="17"/>
+      <c r="AX387" s="17"/>
+      <c r="AY387" s="17"/>
+      <c r="AZ387" s="17"/>
+      <c r="BA387" s="17"/>
+      <c r="BB387" s="17"/>
+      <c r="BC387" s="17"/>
+      <c r="BD387" s="17"/>
+      <c r="BE387" s="17"/>
+      <c r="BF387" s="17"/>
+      <c r="BG387" s="17"/>
+      <c r="BH387" s="17"/>
+      <c r="BI387" s="17"/>
+      <c r="BJ387" s="17"/>
+      <c r="BK387" s="17"/>
+      <c r="BL387" s="17"/>
+      <c r="BM387" s="17"/>
+      <c r="BN387" s="17"/>
+      <c r="BO387" s="17"/>
+      <c r="BP387" s="17"/>
+      <c r="BQ387" s="17"/>
+      <c r="BR387" s="17"/>
+      <c r="BS387" s="17"/>
+      <c r="BT387" s="17"/>
+      <c r="BU387" s="17"/>
+      <c r="BV387" s="17"/>
+    </row>
+    <row r="389" spans="1:74" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A389" s="17"/>
+      <c r="B389" s="17"/>
+      <c r="C389" s="17"/>
+      <c r="D389" s="17"/>
+      <c r="E389" s="17"/>
+      <c r="F389" s="17"/>
+      <c r="G389" s="17"/>
+      <c r="H389" s="17"/>
+      <c r="I389" s="17"/>
+      <c r="J389" s="17"/>
+      <c r="K389" s="17"/>
+      <c r="L389" s="17"/>
+      <c r="M389" s="17"/>
+      <c r="N389" s="17"/>
+      <c r="O389" s="17"/>
+      <c r="P389" s="17"/>
+      <c r="Q389" s="17"/>
+      <c r="R389" s="17"/>
+      <c r="S389" s="17"/>
+      <c r="T389" s="17"/>
+      <c r="U389" s="17"/>
+      <c r="V389" s="17"/>
+      <c r="W389" s="17"/>
+      <c r="X389" s="17"/>
+      <c r="Y389" s="17"/>
+      <c r="Z389" s="17"/>
+      <c r="AA389" s="17"/>
+      <c r="AB389" s="17"/>
+      <c r="AC389" s="17"/>
+      <c r="AD389" s="17"/>
+      <c r="AE389" s="17"/>
+      <c r="AF389" s="17"/>
+      <c r="AG389" s="17"/>
+      <c r="AH389" s="17"/>
+      <c r="AI389" s="17"/>
+      <c r="AJ389" s="17"/>
+      <c r="AK389" s="17"/>
+      <c r="AL389" s="17"/>
+      <c r="AM389" s="17"/>
+      <c r="AN389" s="17"/>
+      <c r="AO389" s="17"/>
+      <c r="AP389" s="17"/>
+      <c r="AQ389" s="17"/>
+      <c r="AR389" s="17"/>
+      <c r="AS389" s="17"/>
+      <c r="AT389" s="17"/>
+      <c r="AU389" s="17"/>
+      <c r="AV389" s="17"/>
+      <c r="AW389" s="17"/>
+      <c r="AX389" s="17"/>
+      <c r="AY389" s="17"/>
+      <c r="AZ389" s="17"/>
+      <c r="BA389" s="17"/>
+      <c r="BB389" s="17"/>
+      <c r="BC389" s="17"/>
+      <c r="BD389" s="17"/>
+      <c r="BE389" s="17"/>
+      <c r="BF389" s="17"/>
+      <c r="BG389" s="17"/>
+      <c r="BH389" s="17"/>
+      <c r="BI389" s="17"/>
+      <c r="BJ389" s="17"/>
+      <c r="BK389" s="17"/>
+      <c r="BL389" s="17"/>
+      <c r="BM389" s="17"/>
+      <c r="BN389" s="17"/>
+      <c r="BO389" s="17"/>
+      <c r="BP389" s="17"/>
+      <c r="BQ389" s="17"/>
+      <c r="BR389" s="17"/>
+      <c r="BS389" s="17"/>
+      <c r="BT389" s="17"/>
+      <c r="BU389" s="17"/>
+      <c r="BV389" s="17"/>
+    </row>
+    <row r="391" spans="1:74" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A391" s="17"/>
+      <c r="B391" s="17"/>
+      <c r="C391" s="17"/>
+      <c r="D391" s="17"/>
+      <c r="E391" s="17"/>
+      <c r="F391" s="17"/>
+      <c r="G391" s="17"/>
+      <c r="H391" s="17"/>
+      <c r="I391" s="17"/>
+      <c r="J391" s="17"/>
+      <c r="K391" s="17"/>
+      <c r="L391" s="17"/>
+      <c r="M391" s="17"/>
+      <c r="N391" s="17"/>
+      <c r="O391" s="17"/>
+      <c r="P391" s="17"/>
+      <c r="Q391" s="17"/>
+      <c r="R391" s="17"/>
+      <c r="S391" s="17"/>
+      <c r="T391" s="17"/>
+      <c r="U391" s="17"/>
+      <c r="V391" s="17"/>
+      <c r="W391" s="17"/>
+      <c r="X391" s="17"/>
+      <c r="Y391" s="17"/>
+      <c r="Z391" s="17"/>
+      <c r="AA391" s="17"/>
+      <c r="AB391" s="17"/>
+      <c r="AC391" s="17"/>
+      <c r="AD391" s="17"/>
+      <c r="AE391" s="17"/>
+      <c r="AF391" s="17"/>
+      <c r="AG391" s="17"/>
+      <c r="AH391" s="17"/>
+      <c r="AI391" s="17"/>
+      <c r="AJ391" s="17"/>
+      <c r="AK391" s="17"/>
+      <c r="AL391" s="17"/>
+      <c r="AM391" s="17"/>
+      <c r="AN391" s="17"/>
+      <c r="AO391" s="17"/>
+      <c r="AP391" s="17"/>
+      <c r="AQ391" s="17"/>
+      <c r="AR391" s="17"/>
+      <c r="AS391" s="17"/>
+      <c r="AT391" s="17"/>
+      <c r="AU391" s="17"/>
+      <c r="AV391" s="17"/>
+      <c r="AW391" s="17"/>
+      <c r="AX391" s="17"/>
+      <c r="AY391" s="17"/>
+      <c r="AZ391" s="17"/>
+      <c r="BA391" s="17"/>
+      <c r="BB391" s="17"/>
+      <c r="BC391" s="17"/>
+      <c r="BD391" s="17"/>
+      <c r="BE391" s="17"/>
+      <c r="BF391" s="17"/>
+      <c r="BG391" s="17"/>
+      <c r="BH391" s="17"/>
+      <c r="BI391" s="17"/>
+      <c r="BJ391" s="17"/>
+      <c r="BK391" s="17"/>
+      <c r="BL391" s="17"/>
+      <c r="BM391" s="17"/>
+      <c r="BN391" s="17"/>
+      <c r="BO391" s="17"/>
+      <c r="BP391" s="17"/>
+      <c r="BQ391" s="17"/>
+      <c r="BR391" s="17"/>
+      <c r="BS391" s="17"/>
+      <c r="BT391" s="17"/>
+      <c r="BU391" s="17"/>
+      <c r="BV391" s="17"/>
+    </row>
+    <row r="436" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A436" s="12"/>
+      <c r="B436" s="12"/>
+      <c r="C436" s="12"/>
+      <c r="D436" s="12"/>
+      <c r="E436" s="12"/>
+      <c r="F436" s="12"/>
+      <c r="G436" s="12"/>
+      <c r="H436" s="12"/>
+      <c r="I436" s="12"/>
+      <c r="J436" s="12"/>
       <c r="K436" s="12"/>
       <c r="L436" s="12"/>
     </row>
@@ -10776,17 +12503,17 @@
       <c r="K439" s="12"/>
       <c r="L439" s="12"/>
     </row>
-    <row r="440" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A440" s="12"/>
-      <c r="B440" s="12"/>
-      <c r="C440" s="12"/>
-      <c r="D440" s="12"/>
-      <c r="E440" s="12"/>
-      <c r="F440" s="12"/>
-      <c r="G440" s="12"/>
-      <c r="H440" s="12"/>
-      <c r="I440" s="12"/>
-      <c r="J440" s="12"/>
+    <row r="440" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A440" s="14"/>
+      <c r="B440" s="14"/>
+      <c r="C440" s="14"/>
+      <c r="D440" s="14"/>
+      <c r="E440" s="14"/>
+      <c r="F440" s="14"/>
+      <c r="G440" s="14"/>
+      <c r="H440" s="14"/>
+      <c r="I440" s="14"/>
+      <c r="J440" s="14"/>
       <c r="K440" s="12"/>
       <c r="L440" s="12"/>
     </row>
@@ -10846,59 +12573,59 @@
       <c r="K444" s="12"/>
       <c r="L444" s="12"/>
     </row>
-    <row r="445" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A445" s="14"/>
-      <c r="B445" s="14"/>
-      <c r="C445" s="14"/>
-      <c r="D445" s="14"/>
-      <c r="E445" s="14"/>
-      <c r="F445" s="14"/>
-      <c r="G445" s="14"/>
-      <c r="H445" s="14"/>
-      <c r="I445" s="14"/>
-      <c r="J445" s="14"/>
+    <row r="445" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A445" s="12"/>
+      <c r="B445" s="12"/>
+      <c r="C445" s="12"/>
+      <c r="D445" s="12"/>
+      <c r="E445" s="12"/>
+      <c r="F445" s="12"/>
+      <c r="G445" s="12"/>
+      <c r="H445" s="12"/>
+      <c r="I445" s="12"/>
+      <c r="J445" s="12"/>
       <c r="K445" s="12"/>
       <c r="L445" s="12"/>
     </row>
-    <row r="446" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A446" s="14"/>
-      <c r="B446" s="14"/>
-      <c r="C446" s="14"/>
-      <c r="D446" s="14"/>
-      <c r="E446" s="14"/>
-      <c r="F446" s="14"/>
-      <c r="G446" s="14"/>
-      <c r="H446" s="14"/>
-      <c r="I446" s="14"/>
-      <c r="J446" s="14"/>
+    <row r="446" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A446" s="12"/>
+      <c r="B446" s="12"/>
+      <c r="C446" s="12"/>
+      <c r="D446" s="12"/>
+      <c r="E446" s="12"/>
+      <c r="F446" s="12"/>
+      <c r="G446" s="12"/>
+      <c r="H446" s="12"/>
+      <c r="I446" s="12"/>
+      <c r="J446" s="12"/>
       <c r="K446" s="12"/>
       <c r="L446" s="12"/>
     </row>
-    <row r="447" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A447" s="14"/>
-      <c r="B447" s="14"/>
-      <c r="C447" s="14"/>
-      <c r="D447" s="14"/>
-      <c r="E447" s="14"/>
-      <c r="F447" s="14"/>
-      <c r="G447" s="14"/>
-      <c r="H447" s="14"/>
-      <c r="I447" s="14"/>
-      <c r="J447" s="14"/>
+    <row r="447" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A447" s="12"/>
+      <c r="B447" s="12"/>
+      <c r="C447" s="12"/>
+      <c r="D447" s="12"/>
+      <c r="E447" s="12"/>
+      <c r="F447" s="12"/>
+      <c r="G447" s="12"/>
+      <c r="H447" s="12"/>
+      <c r="I447" s="12"/>
+      <c r="J447" s="12"/>
       <c r="K447" s="12"/>
       <c r="L447" s="12"/>
     </row>
-    <row r="448" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A448" s="14"/>
-      <c r="B448" s="14"/>
-      <c r="C448" s="14"/>
-      <c r="D448" s="14"/>
-      <c r="E448" s="14"/>
-      <c r="F448" s="14"/>
-      <c r="G448" s="14"/>
-      <c r="H448" s="14"/>
-      <c r="I448" s="14"/>
-      <c r="J448" s="14"/>
+    <row r="448" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A448" s="12"/>
+      <c r="B448" s="12"/>
+      <c r="C448" s="12"/>
+      <c r="D448" s="12"/>
+      <c r="E448" s="12"/>
+      <c r="F448" s="12"/>
+      <c r="G448" s="12"/>
+      <c r="H448" s="12"/>
+      <c r="I448" s="12"/>
+      <c r="J448" s="12"/>
       <c r="K448" s="12"/>
       <c r="L448" s="12"/>
     </row>
@@ -10916,45 +12643,45 @@
       <c r="K449" s="12"/>
       <c r="L449" s="12"/>
     </row>
-    <row r="450" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A450" s="12"/>
-      <c r="B450" s="12"/>
-      <c r="C450" s="12"/>
-      <c r="D450" s="12"/>
-      <c r="E450" s="12"/>
-      <c r="F450" s="12"/>
-      <c r="G450" s="12"/>
-      <c r="H450" s="12"/>
-      <c r="I450" s="12"/>
-      <c r="J450" s="12"/>
+    <row r="450" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A450" s="14"/>
+      <c r="B450" s="14"/>
+      <c r="C450" s="14"/>
+      <c r="D450" s="14"/>
+      <c r="E450" s="14"/>
+      <c r="F450" s="14"/>
+      <c r="G450" s="14"/>
+      <c r="H450" s="14"/>
+      <c r="I450" s="14"/>
+      <c r="J450" s="14"/>
       <c r="K450" s="12"/>
       <c r="L450" s="12"/>
     </row>
-    <row r="451" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A451" s="12"/>
-      <c r="B451" s="12"/>
-      <c r="C451" s="12"/>
-      <c r="D451" s="12"/>
-      <c r="E451" s="12"/>
-      <c r="F451" s="12"/>
-      <c r="G451" s="12"/>
-      <c r="H451" s="12"/>
-      <c r="I451" s="12"/>
-      <c r="J451" s="12"/>
+    <row r="451" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A451" s="14"/>
+      <c r="B451" s="14"/>
+      <c r="C451" s="14"/>
+      <c r="D451" s="14"/>
+      <c r="E451" s="14"/>
+      <c r="F451" s="14"/>
+      <c r="G451" s="14"/>
+      <c r="H451" s="14"/>
+      <c r="I451" s="14"/>
+      <c r="J451" s="14"/>
       <c r="K451" s="12"/>
       <c r="L451" s="12"/>
     </row>
-    <row r="452" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A452" s="12"/>
-      <c r="B452" s="12"/>
-      <c r="C452" s="12"/>
-      <c r="D452" s="12"/>
-      <c r="E452" s="12"/>
-      <c r="F452" s="12"/>
-      <c r="G452" s="12"/>
-      <c r="H452" s="12"/>
-      <c r="I452" s="12"/>
-      <c r="J452" s="12"/>
+    <row r="452" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A452" s="14"/>
+      <c r="B452" s="14"/>
+      <c r="C452" s="14"/>
+      <c r="D452" s="14"/>
+      <c r="E452" s="14"/>
+      <c r="F452" s="14"/>
+      <c r="G452" s="14"/>
+      <c r="H452" s="14"/>
+      <c r="I452" s="14"/>
+      <c r="J452" s="14"/>
       <c r="K452" s="12"/>
       <c r="L452" s="12"/>
     </row>
@@ -11028,55 +12755,55 @@
       <c r="K457" s="12"/>
       <c r="L457" s="12"/>
     </row>
-    <row r="458" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A458" s="14"/>
-      <c r="B458" s="14"/>
-      <c r="C458" s="14"/>
-      <c r="D458" s="14"/>
-      <c r="E458" s="14"/>
-      <c r="F458" s="14"/>
-      <c r="G458" s="14"/>
-      <c r="H458" s="14"/>
-      <c r="I458" s="14"/>
-      <c r="J458" s="14"/>
+    <row r="458" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A458" s="12"/>
+      <c r="B458" s="12"/>
+      <c r="C458" s="12"/>
+      <c r="D458" s="12"/>
+      <c r="E458" s="12"/>
+      <c r="F458" s="12"/>
+      <c r="G458" s="12"/>
+      <c r="H458" s="12"/>
+      <c r="I458" s="12"/>
+      <c r="J458" s="12"/>
       <c r="K458" s="12"/>
       <c r="L458" s="12"/>
     </row>
-    <row r="459" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A459" s="14"/>
-      <c r="B459" s="14"/>
-      <c r="C459" s="14"/>
-      <c r="D459" s="14"/>
-      <c r="E459" s="14"/>
-      <c r="F459" s="14"/>
-      <c r="G459" s="14"/>
-      <c r="H459" s="14"/>
-      <c r="I459" s="14"/>
-      <c r="J459" s="14"/>
+    <row r="459" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A459" s="12"/>
+      <c r="B459" s="12"/>
+      <c r="C459" s="12"/>
+      <c r="D459" s="12"/>
+      <c r="E459" s="12"/>
+      <c r="F459" s="12"/>
+      <c r="G459" s="12"/>
+      <c r="H459" s="12"/>
+      <c r="I459" s="12"/>
+      <c r="J459" s="12"/>
       <c r="K459" s="12"/>
       <c r="L459" s="12"/>
     </row>
-    <row r="460" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="460" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A460" s="12"/>
       <c r="B460" s="12"/>
       <c r="C460" s="12"/>
       <c r="D460" s="12"/>
       <c r="E460" s="12"/>
       <c r="F460" s="12"/>
-      <c r="G460" s="14"/>
-      <c r="H460" s="14"/>
-      <c r="I460" s="14"/>
-      <c r="J460" s="14"/>
+      <c r="G460" s="12"/>
+      <c r="H460" s="12"/>
+      <c r="I460" s="12"/>
+      <c r="J460" s="12"/>
       <c r="K460" s="12"/>
       <c r="L460" s="12"/>
     </row>
     <row r="461" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A461" s="12"/>
-      <c r="B461" s="12"/>
-      <c r="C461" s="12"/>
-      <c r="D461" s="12"/>
-      <c r="E461" s="12"/>
-      <c r="F461" s="12"/>
+      <c r="A461" s="14"/>
+      <c r="B461" s="14"/>
+      <c r="C461" s="14"/>
+      <c r="D461" s="14"/>
+      <c r="E461" s="14"/>
+      <c r="F461" s="14"/>
       <c r="G461" s="14"/>
       <c r="H461" s="14"/>
       <c r="I461" s="14"/>
@@ -11085,12 +12812,12 @@
       <c r="L461" s="12"/>
     </row>
     <row r="462" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A462" s="12"/>
-      <c r="B462" s="12"/>
-      <c r="C462" s="12"/>
-      <c r="D462" s="12"/>
-      <c r="E462" s="12"/>
-      <c r="F462" s="12"/>
+      <c r="A462" s="14"/>
+      <c r="B462" s="14"/>
+      <c r="C462" s="14"/>
+      <c r="D462" s="14"/>
+      <c r="E462" s="14"/>
+      <c r="F462" s="14"/>
       <c r="G462" s="14"/>
       <c r="H462" s="14"/>
       <c r="I462" s="14"/>
@@ -11098,17 +12825,17 @@
       <c r="K462" s="12"/>
       <c r="L462" s="12"/>
     </row>
-    <row r="463" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A463" s="12"/>
-      <c r="B463" s="12"/>
-      <c r="C463" s="12"/>
-      <c r="D463" s="12"/>
-      <c r="E463" s="12"/>
-      <c r="F463" s="12"/>
-      <c r="G463" s="12"/>
-      <c r="H463" s="12"/>
-      <c r="I463" s="12"/>
-      <c r="J463" s="12"/>
+    <row r="463" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A463" s="14"/>
+      <c r="B463" s="14"/>
+      <c r="C463" s="14"/>
+      <c r="D463" s="14"/>
+      <c r="E463" s="14"/>
+      <c r="F463" s="14"/>
+      <c r="G463" s="14"/>
+      <c r="H463" s="14"/>
+      <c r="I463" s="14"/>
+      <c r="J463" s="14"/>
       <c r="K463" s="12"/>
       <c r="L463" s="12"/>
     </row>
@@ -11140,40 +12867,152 @@
       <c r="K465" s="12"/>
       <c r="L465" s="12"/>
     </row>
-    <row r="490" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A490" s="9"/>
-      <c r="B490" s="9"/>
-      <c r="C490" s="9"/>
-      <c r="D490" s="9"/>
-      <c r="E490" s="9"/>
-      <c r="F490" s="9"/>
-      <c r="G490" s="9"/>
-      <c r="H490" s="9"/>
-      <c r="I490" s="9"/>
-      <c r="J490" s="9"/>
-    </row>
-    <row r="492" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A492" t="s">
+    <row r="466" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A466" s="14"/>
+      <c r="B466" s="14"/>
+      <c r="C466" s="14"/>
+      <c r="D466" s="14"/>
+      <c r="E466" s="14"/>
+      <c r="F466" s="14"/>
+      <c r="G466" s="14"/>
+      <c r="H466" s="14"/>
+      <c r="I466" s="14"/>
+      <c r="J466" s="14"/>
+      <c r="K466" s="12"/>
+      <c r="L466" s="12"/>
+    </row>
+    <row r="467" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A467" s="14"/>
+      <c r="B467" s="14"/>
+      <c r="C467" s="14"/>
+      <c r="D467" s="14"/>
+      <c r="E467" s="14"/>
+      <c r="F467" s="14"/>
+      <c r="G467" s="14"/>
+      <c r="H467" s="14"/>
+      <c r="I467" s="14"/>
+      <c r="J467" s="14"/>
+      <c r="K467" s="12"/>
+      <c r="L467" s="12"/>
+    </row>
+    <row r="468" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A468" s="12"/>
+      <c r="B468" s="12"/>
+      <c r="C468" s="12"/>
+      <c r="D468" s="12"/>
+      <c r="E468" s="12"/>
+      <c r="F468" s="12"/>
+      <c r="G468" s="14"/>
+      <c r="H468" s="14"/>
+      <c r="I468" s="14"/>
+      <c r="J468" s="14"/>
+      <c r="K468" s="12"/>
+      <c r="L468" s="12"/>
+    </row>
+    <row r="469" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A469" s="12"/>
+      <c r="B469" s="12"/>
+      <c r="C469" s="12"/>
+      <c r="D469" s="12"/>
+      <c r="E469" s="12"/>
+      <c r="F469" s="12"/>
+      <c r="G469" s="14"/>
+      <c r="H469" s="14"/>
+      <c r="I469" s="14"/>
+      <c r="J469" s="14"/>
+      <c r="K469" s="12"/>
+      <c r="L469" s="12"/>
+    </row>
+    <row r="470" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A470" s="12"/>
+      <c r="B470" s="12"/>
+      <c r="C470" s="12"/>
+      <c r="D470" s="12"/>
+      <c r="E470" s="12"/>
+      <c r="F470" s="12"/>
+      <c r="G470" s="14"/>
+      <c r="H470" s="14"/>
+      <c r="I470" s="14"/>
+      <c r="J470" s="14"/>
+      <c r="K470" s="12"/>
+      <c r="L470" s="12"/>
+    </row>
+    <row r="471" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A471" s="12"/>
+      <c r="B471" s="12"/>
+      <c r="C471" s="12"/>
+      <c r="D471" s="12"/>
+      <c r="E471" s="12"/>
+      <c r="F471" s="12"/>
+      <c r="G471" s="12"/>
+      <c r="H471" s="12"/>
+      <c r="I471" s="12"/>
+      <c r="J471" s="12"/>
+      <c r="K471" s="12"/>
+      <c r="L471" s="12"/>
+    </row>
+    <row r="472" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A472" s="14"/>
+      <c r="B472" s="14"/>
+      <c r="C472" s="14"/>
+      <c r="D472" s="14"/>
+      <c r="E472" s="14"/>
+      <c r="F472" s="14"/>
+      <c r="G472" s="14"/>
+      <c r="H472" s="14"/>
+      <c r="I472" s="14"/>
+      <c r="J472" s="14"/>
+      <c r="K472" s="12"/>
+      <c r="L472" s="12"/>
+    </row>
+    <row r="473" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A473" s="14"/>
+      <c r="B473" s="14"/>
+      <c r="C473" s="14"/>
+      <c r="D473" s="14"/>
+      <c r="E473" s="14"/>
+      <c r="F473" s="14"/>
+      <c r="G473" s="14"/>
+      <c r="H473" s="14"/>
+      <c r="I473" s="14"/>
+      <c r="J473" s="14"/>
+      <c r="K473" s="12"/>
+      <c r="L473" s="12"/>
+    </row>
+    <row r="498" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A498" s="9"/>
+      <c r="B498" s="9"/>
+      <c r="C498" s="9"/>
+      <c r="D498" s="9"/>
+      <c r="E498" s="9"/>
+      <c r="F498" s="9"/>
+      <c r="G498" s="9"/>
+      <c r="H498" s="9"/>
+      <c r="I498" s="9"/>
+      <c r="J498" s="9"/>
+    </row>
+    <row r="500" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A500" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="493" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A493" t="s">
+    <row r="501" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A501" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="494" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A494" t="s">
+    <row r="502" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A502" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="495" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A495" t="s">
+    <row r="503" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A503" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="496" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A496" t="s">
+    <row r="504" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A504" t="s">
         <v>125</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Bunny Edits Plus Minotaur Roar
</commit_message>
<xml_diff>
--- a/Documents/AssetList-Planning.xlsx
+++ b/Documents/AssetList-Planning.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18067"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Enra\Pictures\Orphanage\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deesv_000\Desktop\Orphanage\Orphanage\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="765" uniqueCount="459">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="782" uniqueCount="476">
   <si>
     <t>Planning</t>
   </si>
@@ -1122,9 +1122,6 @@
     <t>Shield Block</t>
   </si>
   <si>
-    <t>Minotaures</t>
-  </si>
-  <si>
     <t>Footsteps</t>
   </si>
   <si>
@@ -1221,9 +1218,6 @@
     <t>7S-INT-ShieldBlock</t>
   </si>
   <si>
-    <t>7S-CHAR-Minotaures</t>
-  </si>
-  <si>
     <t>7S-CHAR-Footsteps</t>
   </si>
   <si>
@@ -1402,12 +1396,69 @@
   </si>
   <si>
     <t>CoinGlimmer</t>
+  </si>
+  <si>
+    <t>Minotaur Roar</t>
+  </si>
+  <si>
+    <t>Minotaur Slash</t>
+  </si>
+  <si>
+    <t>Minotaur AxeToGround</t>
+  </si>
+  <si>
+    <t>Minotaur Grunt</t>
+  </si>
+  <si>
+    <t>Minotaur Walk</t>
+  </si>
+  <si>
+    <t>Minotaur Hit</t>
+  </si>
+  <si>
+    <t>Minotaur Death</t>
+  </si>
+  <si>
+    <t>Minotaur Stagger</t>
+  </si>
+  <si>
+    <t>7S-CHAR-MinotaurRoar</t>
+  </si>
+  <si>
+    <t>7S-CHAR-MinotaurATG</t>
+  </si>
+  <si>
+    <t>7S-CHAR-MinotaurSlash</t>
+  </si>
+  <si>
+    <t>7S-CHAR-MinotaurGrunt</t>
+  </si>
+  <si>
+    <t>7S-CHAR-MinotaurWalk</t>
+  </si>
+  <si>
+    <t>7S-CHAR-MinotaurHit</t>
+  </si>
+  <si>
+    <t>7S-CHAR-MinotaurDeath</t>
+  </si>
+  <si>
+    <t>7S-CHAR-MinotaurBChrg</t>
+  </si>
+  <si>
+    <t>7S-CHAR-MinotaurStggr</t>
+  </si>
+  <si>
+    <t>Minotaur Charge Sprint</t>
+  </si>
+  <si>
+    <t>Minotaur Charge Grunt</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1947,7 +1998,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BI93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U40" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="U56" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="AP76" sqref="AP76"/>
     </sheetView>
   </sheetViews>
@@ -2156,7 +2207,7 @@
       </c>
       <c r="AD7" s="27"/>
       <c r="AE7" s="9" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="AK7" s="27"/>
       <c r="AL7" s="9" t="s">
@@ -2311,7 +2362,7 @@
       </c>
       <c r="P18" s="27"/>
       <c r="Q18" s="9" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="W18" s="27"/>
       <c r="X18" s="9" t="s">
@@ -2323,7 +2374,7 @@
       </c>
       <c r="AK18" s="27"/>
       <c r="AL18" s="9" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="AR18" s="27"/>
       <c r="AY18" s="27"/>
@@ -2339,15 +2390,15 @@
       <c r="P19" s="27"/>
       <c r="W19" s="27"/>
       <c r="X19" s="9" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="AD19" s="27"/>
       <c r="AE19" s="9" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="AK19" s="27"/>
       <c r="AL19" s="9" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="AR19" s="27"/>
       <c r="AY19" s="27"/>
@@ -2490,7 +2541,7 @@
       </c>
       <c r="AD29" s="27"/>
       <c r="AE29" s="9" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="AK29" s="27"/>
       <c r="AR29" s="27"/>
@@ -2512,7 +2563,7 @@
       </c>
       <c r="P30" s="27"/>
       <c r="Q30" s="9" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="W30" s="27"/>
       <c r="X30" s="9" t="s">
@@ -2520,7 +2571,7 @@
       </c>
       <c r="AD30" s="27"/>
       <c r="AE30" s="9" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="AK30" s="27"/>
       <c r="AR30" s="27"/>
@@ -2544,7 +2595,7 @@
       </c>
       <c r="AD31" s="27"/>
       <c r="AE31" s="9" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="AK31" s="27"/>
       <c r="AR31" s="27"/>
@@ -2662,7 +2713,7 @@
       </c>
       <c r="P40" s="27"/>
       <c r="Q40" s="9" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="S40" s="9" t="s">
         <v>344</v>
@@ -2680,11 +2731,11 @@
         <v>100</v>
       </c>
       <c r="AO40" s="9" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="AR40" s="27"/>
       <c r="AS40" s="9" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="AY40" s="27"/>
       <c r="BF40" s="27"/>
@@ -2837,15 +2888,15 @@
       </c>
       <c r="W51" s="27"/>
       <c r="X51" s="9" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="AD51" s="27"/>
       <c r="AE51" s="9" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="AK51" s="27"/>
       <c r="AL51" s="9" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="AR51" s="27"/>
       <c r="AY51" s="27"/>
@@ -2868,7 +2919,7 @@
       <c r="W52" s="27"/>
       <c r="AD52" s="27"/>
       <c r="AE52" s="9" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="AK52" s="27"/>
       <c r="AR52" s="27"/>
@@ -2883,7 +2934,7 @@
       <c r="W53" s="27"/>
       <c r="AD53" s="27"/>
       <c r="AE53" s="9" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="AK53" s="27"/>
       <c r="AR53" s="27"/>
@@ -2999,19 +3050,19 @@
       </c>
       <c r="W62" s="27"/>
       <c r="X62" s="9" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="AD62" s="27"/>
       <c r="AE62" s="9" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="AK62" s="27"/>
       <c r="AL62" s="9" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="AR62" s="27"/>
       <c r="AS62" s="9" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="AY62" s="27"/>
       <c r="BF62" s="27"/>
@@ -3026,7 +3077,7 @@
       <c r="AK63" s="27"/>
       <c r="AR63" s="27"/>
       <c r="AS63" s="9" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="AY63" s="27"/>
       <c r="BF63" s="27"/>
@@ -3148,32 +3199,32 @@
         <v>339</v>
       </c>
       <c r="S73" s="9" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="T73" s="9" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="W73" s="27"/>
       <c r="X73" s="9" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="AA73" s="9" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="AD73" s="27"/>
       <c r="AE73" s="9" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="AH73" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="AK73" s="27"/>
       <c r="AL73" s="9" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="AR73" s="27"/>
       <c r="AS73" s="9" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="AY73" s="27"/>
       <c r="BF73" s="27"/>
@@ -3188,21 +3239,21 @@
       <c r="P74" s="27"/>
       <c r="W74" s="27"/>
       <c r="X74" s="9" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="AA74" s="9" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="AD74" s="27"/>
       <c r="AE74" s="9" t="s">
+        <v>429</v>
+      </c>
+      <c r="AH74" s="9" t="s">
         <v>431</v>
-      </c>
-      <c r="AH74" s="9" t="s">
-        <v>433</v>
       </c>
       <c r="AK74" s="27"/>
       <c r="AL74" s="9" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="AR74" s="27"/>
       <c r="AS74" s="9" t="s">
@@ -3214,19 +3265,19 @@
     </row>
     <row r="75" spans="1:59" ht="15.75" x14ac:dyDescent="0.25">
       <c r="AE75" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="AH75" s="9" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="AL75" s="9" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="AS75" s="9"/>
     </row>
     <row r="76" spans="1:59" ht="15.75" x14ac:dyDescent="0.25">
       <c r="AH76" s="9" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="AL76" s="9"/>
       <c r="AS76" s="9"/>
@@ -3256,7 +3307,7 @@
       </c>
       <c r="AR84" s="27"/>
       <c r="AS84" s="9" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="AY84" s="27"/>
       <c r="BF84" s="27"/>
@@ -3381,10 +3432,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:QF496"/>
+  <dimension ref="A1:QF506"/>
   <sheetViews>
-    <sheetView topLeftCell="A301" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A315" sqref="A315:XFD315"/>
+    <sheetView tabSelected="1" topLeftCell="A335" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A355" sqref="A355"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3530,7 +3581,7 @@
         <v>19</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>20</v>
@@ -5779,7 +5830,7 @@
         <v>340</v>
       </c>
       <c r="D287" s="9" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="I287" s="9" t="s">
         <v>50</v>
@@ -5794,7 +5845,7 @@
         <v>341</v>
       </c>
       <c r="D289" s="9" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="I289" s="9" t="s">
         <v>50</v>
@@ -5803,10 +5854,10 @@
     <row r="290" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="291" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A291" s="9" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D291" s="9" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="I291" s="9" t="s">
         <v>39</v>
@@ -5818,10 +5869,10 @@
     <row r="292" spans="1:10" s="17" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="293" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A293" s="9" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="D293" s="9" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="I293" s="9" t="s">
         <v>39</v>
@@ -5836,7 +5887,7 @@
         <v>343</v>
       </c>
       <c r="D295" s="9" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="I295" s="9" t="s">
         <v>39</v>
@@ -5851,7 +5902,7 @@
         <v>345</v>
       </c>
       <c r="D297" s="9" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="I297" s="9" t="s">
         <v>39</v>
@@ -5866,7 +5917,7 @@
         <v>346</v>
       </c>
       <c r="D299" s="9" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="I299" s="9" t="s">
         <v>39</v>
@@ -5881,7 +5932,7 @@
         <v>347</v>
       </c>
       <c r="D301" s="9" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="I301" s="9" t="s">
         <v>39</v>
@@ -5899,7 +5950,7 @@
         <v>302</v>
       </c>
       <c r="D303" s="9" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="I303" s="9" t="s">
         <v>50</v>
@@ -5917,7 +5968,7 @@
         <v>350</v>
       </c>
       <c r="D305" s="9" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="I305" s="9" t="s">
         <v>50</v>
@@ -5929,7 +5980,7 @@
         <v>355</v>
       </c>
       <c r="D307" s="9" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="I307" s="9" t="s">
         <v>50</v>
@@ -5941,7 +5992,7 @@
         <v>351</v>
       </c>
       <c r="D309" s="9" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="I309" s="9" t="s">
         <v>39</v>
@@ -6405,7 +6456,7 @@
         <v>352</v>
       </c>
       <c r="D311" s="9" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="I311" s="9" t="s">
         <v>50</v>
@@ -6869,7 +6920,7 @@
         <v>353</v>
       </c>
       <c r="D313" s="9" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="I313" s="9" t="s">
         <v>50</v>
@@ -7330,13 +7381,13 @@
     </row>
     <row r="315" spans="1:448" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A315" s="9" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="B315" s="9" t="s">
         <v>354</v>
       </c>
       <c r="D315" s="9" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="I315" s="9" t="s">
         <v>39</v>
@@ -7797,10 +7848,10 @@
     </row>
     <row r="317" spans="1:448" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A317" s="9" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="D317" s="9" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="I317" s="9" t="s">
         <v>50</v>
@@ -8261,10 +8312,10 @@
     </row>
     <row r="319" spans="1:448" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A319" s="14" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D319" s="14" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="I319" s="14" t="s">
         <v>39</v>
@@ -8725,10 +8776,10 @@
     </row>
     <row r="321" spans="1:448" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A321" s="14" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="D321" s="14" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="I321" s="14" t="s">
         <v>50</v>
@@ -9186,10 +9237,10 @@
     </row>
     <row r="323" spans="1:448" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A323" s="14" t="s">
+        <v>418</v>
+      </c>
+      <c r="D323" s="14" t="s">
         <v>420</v>
-      </c>
-      <c r="D323" s="14" t="s">
-        <v>422</v>
       </c>
       <c r="I323" s="14" t="s">
         <v>50</v>
@@ -9650,10 +9701,10 @@
     </row>
     <row r="325" spans="1:448" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A325" s="14" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="D325" s="14" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="I325" s="14" t="s">
         <v>39</v>
@@ -10124,7 +10175,7 @@
         <v>357</v>
       </c>
       <c r="D330" s="14" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="I330" s="14" t="s">
         <v>39</v>
@@ -10214,7 +10265,7 @@
         <v>358</v>
       </c>
       <c r="D332" s="14" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="I332" s="14" t="s">
         <v>50</v>
@@ -10301,7 +10352,7 @@
         <v>359</v>
       </c>
       <c r="D334" s="14" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="I334" s="14" t="s">
         <v>50</v>
@@ -10388,7 +10439,7 @@
         <v>360</v>
       </c>
       <c r="D336" s="14" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="I336" s="14" t="s">
         <v>50</v>
@@ -10475,7 +10526,7 @@
         <v>361</v>
       </c>
       <c r="D338" s="14" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="I338" s="14" t="s">
         <v>39</v>
@@ -10565,7 +10616,7 @@
         <v>362</v>
       </c>
       <c r="D340" s="14" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="I340" s="14" t="s">
         <v>50</v>
@@ -10652,7 +10703,7 @@
         <v>363</v>
       </c>
       <c r="D342" s="14" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="I342" s="14" t="s">
         <v>50</v>
@@ -10739,7 +10790,7 @@
         <v>364</v>
       </c>
       <c r="D344" s="14" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="I344" s="14" t="s">
         <v>50</v>
@@ -10821,25 +10872,95 @@
       <c r="BU345" s="17"/>
       <c r="BV345" s="17"/>
     </row>
-    <row r="346" spans="1:74" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A346" s="14" t="s">
-        <v>365</v>
-      </c>
-      <c r="D346" s="14" t="s">
-        <v>398</v>
-      </c>
-      <c r="I346" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="J346" s="14" t="s">
-        <v>428</v>
-      </c>
+    <row r="346" spans="1:74" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A346" s="17" t="s">
+        <v>459</v>
+      </c>
+      <c r="B346" s="17"/>
+      <c r="C346" s="17"/>
+      <c r="D346" s="17" t="s">
+        <v>466</v>
+      </c>
+      <c r="E346" s="17"/>
+      <c r="F346" s="17"/>
+      <c r="G346" s="17"/>
+      <c r="H346" s="17"/>
+      <c r="I346" s="17"/>
+      <c r="J346" s="17"/>
+      <c r="K346" s="17"/>
+      <c r="L346" s="17"/>
+      <c r="M346" s="17"/>
+      <c r="N346" s="17"/>
+      <c r="O346" s="17"/>
+      <c r="P346" s="17"/>
+      <c r="Q346" s="17"/>
+      <c r="R346" s="17"/>
+      <c r="S346" s="17"/>
+      <c r="T346" s="17"/>
+      <c r="U346" s="17"/>
+      <c r="V346" s="17"/>
+      <c r="W346" s="17"/>
+      <c r="X346" s="17"/>
+      <c r="Y346" s="17"/>
+      <c r="Z346" s="17"/>
+      <c r="AA346" s="17"/>
+      <c r="AB346" s="17"/>
+      <c r="AC346" s="17"/>
+      <c r="AD346" s="17"/>
+      <c r="AE346" s="17"/>
+      <c r="AF346" s="17"/>
+      <c r="AG346" s="17"/>
+      <c r="AH346" s="17"/>
+      <c r="AI346" s="17"/>
+      <c r="AJ346" s="17"/>
+      <c r="AK346" s="17"/>
+      <c r="AL346" s="17"/>
+      <c r="AM346" s="17"/>
+      <c r="AN346" s="17"/>
+      <c r="AO346" s="17"/>
+      <c r="AP346" s="17"/>
+      <c r="AQ346" s="17"/>
+      <c r="AR346" s="17"/>
+      <c r="AS346" s="17"/>
+      <c r="AT346" s="17"/>
+      <c r="AU346" s="17"/>
+      <c r="AV346" s="17"/>
+      <c r="AW346" s="17"/>
+      <c r="AX346" s="17"/>
+      <c r="AY346" s="17"/>
+      <c r="AZ346" s="17"/>
+      <c r="BA346" s="17"/>
+      <c r="BB346" s="17"/>
+      <c r="BC346" s="17"/>
+      <c r="BD346" s="17"/>
+      <c r="BE346" s="17"/>
+      <c r="BF346" s="17"/>
+      <c r="BG346" s="17"/>
+      <c r="BH346" s="17"/>
+      <c r="BI346" s="17"/>
+      <c r="BJ346" s="17"/>
+      <c r="BK346" s="17"/>
+      <c r="BL346" s="17"/>
+      <c r="BM346" s="17"/>
+      <c r="BN346" s="17"/>
+      <c r="BO346" s="17"/>
+      <c r="BP346" s="17"/>
+      <c r="BQ346" s="17"/>
+      <c r="BR346" s="17"/>
+      <c r="BS346" s="17"/>
+      <c r="BT346" s="17"/>
+      <c r="BU346" s="17"/>
+      <c r="BV346" s="17"/>
     </row>
     <row r="347" spans="1:74" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A347" s="17"/>
+      <c r="A347" s="17" t="s">
+        <v>458</v>
+      </c>
       <c r="B347" s="17"/>
       <c r="C347" s="17"/>
-      <c r="D347" s="17"/>
+      <c r="D347" s="17" t="s">
+        <v>467</v>
+      </c>
       <c r="E347" s="17"/>
       <c r="F347" s="17"/>
       <c r="G347" s="17"/>
@@ -10911,380 +11032,74 @@
       <c r="BU347" s="17"/>
       <c r="BV347" s="17"/>
     </row>
-    <row r="348" spans="1:74" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A348" s="9" t="s">
-        <v>366</v>
-      </c>
-      <c r="D348" s="9" t="s">
-        <v>399</v>
-      </c>
-      <c r="I348" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="J348" s="9" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="349" spans="1:74" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A349" s="17"/>
-      <c r="B349" s="17"/>
-      <c r="C349" s="17"/>
-      <c r="D349" s="17"/>
-      <c r="E349" s="17"/>
-      <c r="F349" s="17"/>
-      <c r="G349" s="17"/>
-      <c r="H349" s="17"/>
-      <c r="I349" s="17"/>
-      <c r="J349" s="17"/>
-      <c r="K349" s="17"/>
-      <c r="L349" s="17"/>
-      <c r="M349" s="17"/>
-      <c r="N349" s="17"/>
-      <c r="O349" s="17"/>
-      <c r="P349" s="17"/>
-      <c r="Q349" s="17"/>
-      <c r="R349" s="17"/>
-      <c r="S349" s="17"/>
-      <c r="T349" s="17"/>
-      <c r="U349" s="17"/>
-      <c r="V349" s="17"/>
-      <c r="W349" s="17"/>
-      <c r="X349" s="17"/>
-      <c r="Y349" s="17"/>
-      <c r="Z349" s="17"/>
-      <c r="AA349" s="17"/>
-      <c r="AB349" s="17"/>
-      <c r="AC349" s="17"/>
-      <c r="AD349" s="17"/>
-      <c r="AE349" s="17"/>
-      <c r="AF349" s="17"/>
-      <c r="AG349" s="17"/>
-      <c r="AH349" s="17"/>
-      <c r="AI349" s="17"/>
-      <c r="AJ349" s="17"/>
-      <c r="AK349" s="17"/>
-      <c r="AL349" s="17"/>
-      <c r="AM349" s="17"/>
-      <c r="AN349" s="17"/>
-      <c r="AO349" s="17"/>
-      <c r="AP349" s="17"/>
-      <c r="AQ349" s="17"/>
-      <c r="AR349" s="17"/>
-      <c r="AS349" s="17"/>
-      <c r="AT349" s="17"/>
-      <c r="AU349" s="17"/>
-      <c r="AV349" s="17"/>
-      <c r="AW349" s="17"/>
-      <c r="AX349" s="17"/>
-      <c r="AY349" s="17"/>
-      <c r="AZ349" s="17"/>
-      <c r="BA349" s="17"/>
-      <c r="BB349" s="17"/>
-      <c r="BC349" s="17"/>
-      <c r="BD349" s="17"/>
-      <c r="BE349" s="17"/>
-      <c r="BF349" s="17"/>
-      <c r="BG349" s="17"/>
-      <c r="BH349" s="17"/>
-      <c r="BI349" s="17"/>
-      <c r="BJ349" s="17"/>
-      <c r="BK349" s="17"/>
-      <c r="BL349" s="17"/>
-      <c r="BM349" s="17"/>
-      <c r="BN349" s="17"/>
-      <c r="BO349" s="17"/>
-      <c r="BP349" s="17"/>
-      <c r="BQ349" s="17"/>
-      <c r="BR349" s="17"/>
-      <c r="BS349" s="17"/>
-      <c r="BT349" s="17"/>
-      <c r="BU349" s="17"/>
-      <c r="BV349" s="17"/>
-    </row>
-    <row r="350" spans="1:74" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A350" s="9" t="s">
-        <v>367</v>
-      </c>
-      <c r="D350" s="9" t="s">
-        <v>400</v>
-      </c>
-      <c r="I350" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="J350" s="9" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="351" spans="1:74" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A351" s="17"/>
-      <c r="B351" s="17"/>
-      <c r="C351" s="17"/>
-      <c r="D351" s="17"/>
-      <c r="E351" s="17"/>
-      <c r="F351" s="17"/>
-      <c r="G351" s="17"/>
-      <c r="H351" s="17"/>
-      <c r="I351" s="17"/>
-      <c r="J351" s="17"/>
-      <c r="K351" s="17"/>
-      <c r="L351" s="17"/>
-      <c r="M351" s="17"/>
-      <c r="N351" s="17"/>
-      <c r="O351" s="17"/>
-      <c r="P351" s="17"/>
-      <c r="Q351" s="17"/>
-      <c r="R351" s="17"/>
-      <c r="S351" s="17"/>
-      <c r="T351" s="17"/>
-      <c r="U351" s="17"/>
-      <c r="V351" s="17"/>
-      <c r="W351" s="17"/>
-      <c r="X351" s="17"/>
-      <c r="Y351" s="17"/>
-      <c r="Z351" s="17"/>
-      <c r="AA351" s="17"/>
-      <c r="AB351" s="17"/>
-      <c r="AC351" s="17"/>
-      <c r="AD351" s="17"/>
-      <c r="AE351" s="17"/>
-      <c r="AF351" s="17"/>
-      <c r="AG351" s="17"/>
-      <c r="AH351" s="17"/>
-      <c r="AI351" s="17"/>
-      <c r="AJ351" s="17"/>
-      <c r="AK351" s="17"/>
-      <c r="AL351" s="17"/>
-      <c r="AM351" s="17"/>
-      <c r="AN351" s="17"/>
-      <c r="AO351" s="17"/>
-      <c r="AP351" s="17"/>
-      <c r="AQ351" s="17"/>
-      <c r="AR351" s="17"/>
-      <c r="AS351" s="17"/>
-      <c r="AT351" s="17"/>
-      <c r="AU351" s="17"/>
-      <c r="AV351" s="17"/>
-      <c r="AW351" s="17"/>
-      <c r="AX351" s="17"/>
-      <c r="AY351" s="17"/>
-      <c r="AZ351" s="17"/>
-      <c r="BA351" s="17"/>
-      <c r="BB351" s="17"/>
-      <c r="BC351" s="17"/>
-      <c r="BD351" s="17"/>
-      <c r="BE351" s="17"/>
-      <c r="BF351" s="17"/>
-      <c r="BG351" s="17"/>
-      <c r="BH351" s="17"/>
-      <c r="BI351" s="17"/>
-      <c r="BJ351" s="17"/>
-      <c r="BK351" s="17"/>
-      <c r="BL351" s="17"/>
-      <c r="BM351" s="17"/>
-      <c r="BN351" s="17"/>
-      <c r="BO351" s="17"/>
-      <c r="BP351" s="17"/>
-      <c r="BQ351" s="17"/>
-      <c r="BR351" s="17"/>
-      <c r="BS351" s="17"/>
-      <c r="BT351" s="17"/>
-      <c r="BU351" s="17"/>
-      <c r="BV351" s="17"/>
-    </row>
-    <row r="352" spans="1:74" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A352" s="9" t="s">
-        <v>368</v>
-      </c>
-      <c r="B352" s="9" t="s">
-        <v>302</v>
-      </c>
-      <c r="D352" s="9" t="s">
-        <v>401</v>
-      </c>
-      <c r="I352" s="9" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="353" spans="1:74" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A353" s="17"/>
-      <c r="B353" s="17"/>
-      <c r="C353" s="17"/>
-      <c r="D353" s="17"/>
-      <c r="E353" s="17"/>
-      <c r="F353" s="17"/>
-      <c r="G353" s="17"/>
-      <c r="H353" s="17"/>
-      <c r="I353" s="17"/>
-      <c r="J353" s="17"/>
-      <c r="K353" s="17"/>
-      <c r="L353" s="17"/>
-      <c r="M353" s="17"/>
-      <c r="N353" s="17"/>
-      <c r="O353" s="17"/>
-      <c r="P353" s="17"/>
-      <c r="Q353" s="17"/>
-      <c r="R353" s="17"/>
-      <c r="S353" s="17"/>
-      <c r="T353" s="17"/>
-      <c r="U353" s="17"/>
-      <c r="V353" s="17"/>
-      <c r="W353" s="17"/>
-      <c r="X353" s="17"/>
-      <c r="Y353" s="17"/>
-      <c r="Z353" s="17"/>
-      <c r="AA353" s="17"/>
-      <c r="AB353" s="17"/>
-      <c r="AC353" s="17"/>
-      <c r="AD353" s="17"/>
-      <c r="AE353" s="17"/>
-      <c r="AF353" s="17"/>
-      <c r="AG353" s="17"/>
-      <c r="AH353" s="17"/>
-      <c r="AI353" s="17"/>
-      <c r="AJ353" s="17"/>
-      <c r="AK353" s="17"/>
-      <c r="AL353" s="17"/>
-      <c r="AM353" s="17"/>
-      <c r="AN353" s="17"/>
-      <c r="AO353" s="17"/>
-      <c r="AP353" s="17"/>
-      <c r="AQ353" s="17"/>
-      <c r="AR353" s="17"/>
-      <c r="AS353" s="17"/>
-      <c r="AT353" s="17"/>
-      <c r="AU353" s="17"/>
-      <c r="AV353" s="17"/>
-      <c r="AW353" s="17"/>
-      <c r="AX353" s="17"/>
-      <c r="AY353" s="17"/>
-      <c r="AZ353" s="17"/>
-      <c r="BA353" s="17"/>
-      <c r="BB353" s="17"/>
-      <c r="BC353" s="17"/>
-      <c r="BD353" s="17"/>
-      <c r="BE353" s="17"/>
-      <c r="BF353" s="17"/>
-      <c r="BG353" s="17"/>
-      <c r="BH353" s="17"/>
-      <c r="BI353" s="17"/>
-      <c r="BJ353" s="17"/>
-      <c r="BK353" s="17"/>
-      <c r="BL353" s="17"/>
-      <c r="BM353" s="17"/>
-      <c r="BN353" s="17"/>
-      <c r="BO353" s="17"/>
-      <c r="BP353" s="17"/>
-      <c r="BQ353" s="17"/>
-      <c r="BR353" s="17"/>
-      <c r="BS353" s="17"/>
-      <c r="BT353" s="17"/>
-      <c r="BU353" s="17"/>
-      <c r="BV353" s="17"/>
-    </row>
-    <row r="354" spans="1:74" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A354" s="9" t="s">
-        <v>369</v>
-      </c>
-      <c r="D354" s="9" t="s">
-        <v>402</v>
-      </c>
-      <c r="I354" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="J354" s="9" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="355" spans="1:74" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A355" s="17"/>
-      <c r="B355" s="17"/>
-      <c r="C355" s="17"/>
-      <c r="D355" s="17"/>
-      <c r="E355" s="17"/>
-      <c r="F355" s="17"/>
-      <c r="G355" s="17"/>
-      <c r="H355" s="17"/>
-      <c r="I355" s="17"/>
-      <c r="J355" s="17"/>
-      <c r="K355" s="17"/>
-      <c r="L355" s="17"/>
-      <c r="M355" s="17"/>
-      <c r="N355" s="17"/>
-      <c r="O355" s="17"/>
-      <c r="P355" s="17"/>
-      <c r="Q355" s="17"/>
-      <c r="R355" s="17"/>
-      <c r="S355" s="17"/>
-      <c r="T355" s="17"/>
-      <c r="U355" s="17"/>
-      <c r="V355" s="17"/>
-      <c r="W355" s="17"/>
-      <c r="X355" s="17"/>
-      <c r="Y355" s="17"/>
-      <c r="Z355" s="17"/>
-      <c r="AA355" s="17"/>
-      <c r="AB355" s="17"/>
-      <c r="AC355" s="17"/>
-      <c r="AD355" s="17"/>
-      <c r="AE355" s="17"/>
-      <c r="AF355" s="17"/>
-      <c r="AG355" s="17"/>
-      <c r="AH355" s="17"/>
-      <c r="AI355" s="17"/>
-      <c r="AJ355" s="17"/>
-      <c r="AK355" s="17"/>
-      <c r="AL355" s="17"/>
-      <c r="AM355" s="17"/>
-      <c r="AN355" s="17"/>
-      <c r="AO355" s="17"/>
-      <c r="AP355" s="17"/>
-      <c r="AQ355" s="17"/>
-      <c r="AR355" s="17"/>
-      <c r="AS355" s="17"/>
-      <c r="AT355" s="17"/>
-      <c r="AU355" s="17"/>
-      <c r="AV355" s="17"/>
-      <c r="AW355" s="17"/>
-      <c r="AX355" s="17"/>
-      <c r="AY355" s="17"/>
-      <c r="AZ355" s="17"/>
-      <c r="BA355" s="17"/>
-      <c r="BB355" s="17"/>
-      <c r="BC355" s="17"/>
-      <c r="BD355" s="17"/>
-      <c r="BE355" s="17"/>
-      <c r="BF355" s="17"/>
-      <c r="BG355" s="17"/>
-      <c r="BH355" s="17"/>
-      <c r="BI355" s="17"/>
-      <c r="BJ355" s="17"/>
-      <c r="BK355" s="17"/>
-      <c r="BL355" s="17"/>
-      <c r="BM355" s="17"/>
-      <c r="BN355" s="17"/>
-      <c r="BO355" s="17"/>
-      <c r="BP355" s="17"/>
-      <c r="BQ355" s="17"/>
-      <c r="BR355" s="17"/>
-      <c r="BS355" s="17"/>
-      <c r="BT355" s="17"/>
-      <c r="BU355" s="17"/>
-      <c r="BV355" s="17"/>
-    </row>
-    <row r="356" spans="1:74" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A356" s="9" t="s">
-        <v>370</v>
-      </c>
-      <c r="D356" s="9" t="s">
-        <v>403</v>
-      </c>
-      <c r="I356" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="J356" s="9" t="s">
-        <v>293</v>
-      </c>
-    </row>
+    <row r="348" spans="1:74" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A348" s="14" t="s">
+        <v>457</v>
+      </c>
+      <c r="D348" s="14" t="s">
+        <v>465</v>
+      </c>
+      <c r="I348" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="J348" s="14" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="349" spans="1:74" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A349" s="14" t="s">
+        <v>460</v>
+      </c>
+      <c r="D349" s="14" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="350" spans="1:74" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A350" s="14" t="s">
+        <v>461</v>
+      </c>
+      <c r="D350" s="14" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="351" spans="1:74" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A351" s="14" t="s">
+        <v>462</v>
+      </c>
+      <c r="D351" s="14" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="352" spans="1:74" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A352" s="14" t="s">
+        <v>463</v>
+      </c>
+      <c r="D352" s="14" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="353" spans="1:74" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A353" s="14" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="354" spans="1:74" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A354" s="14" t="s">
+        <v>475</v>
+      </c>
+      <c r="D354" s="14" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="355" spans="1:74" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A355" s="14" t="s">
+        <v>464</v>
+      </c>
+      <c r="D355" s="14" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="356" spans="1:74" s="14" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="357" spans="1:74" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A357" s="17"/>
       <c r="B357" s="17"/>
@@ -11363,13 +11178,16 @@
     </row>
     <row r="358" spans="1:74" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A358" s="9" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="D358" s="9" t="s">
-        <v>404</v>
+        <v>397</v>
       </c>
       <c r="I358" s="9" t="s">
-        <v>50</v>
+        <v>39</v>
+      </c>
+      <c r="J358" s="9" t="s">
+        <v>426</v>
       </c>
     </row>
     <row r="359" spans="1:74" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -11450,13 +11268,16 @@
     </row>
     <row r="360" spans="1:74" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A360" s="9" t="s">
-        <v>342</v>
+        <v>366</v>
       </c>
       <c r="D360" s="9" t="s">
-        <v>405</v>
+        <v>398</v>
       </c>
       <c r="I360" s="9" t="s">
-        <v>50</v>
+        <v>39</v>
+      </c>
+      <c r="J360" s="9" t="s">
+        <v>293</v>
       </c>
     </row>
     <row r="361" spans="1:74" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -11537,10 +11358,13 @@
     </row>
     <row r="362" spans="1:74" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A362" s="9" t="s">
-        <v>372</v>
+        <v>367</v>
+      </c>
+      <c r="B362" s="9" t="s">
+        <v>302</v>
       </c>
       <c r="D362" s="9" t="s">
-        <v>406</v>
+        <v>399</v>
       </c>
       <c r="I362" s="9" t="s">
         <v>50</v>
@@ -11624,13 +11448,16 @@
     </row>
     <row r="364" spans="1:74" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A364" s="9" t="s">
-        <v>410</v>
+        <v>368</v>
       </c>
       <c r="D364" s="9" t="s">
-        <v>411</v>
+        <v>400</v>
       </c>
       <c r="I364" s="9" t="s">
-        <v>50</v>
+        <v>39</v>
+      </c>
+      <c r="J364" s="9" t="s">
+        <v>293</v>
       </c>
     </row>
     <row r="365" spans="1:74" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -11711,13 +11538,16 @@
     </row>
     <row r="366" spans="1:74" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A366" s="9" t="s">
-        <v>412</v>
+        <v>369</v>
       </c>
       <c r="D366" s="9" t="s">
-        <v>413</v>
+        <v>401</v>
       </c>
       <c r="I366" s="9" t="s">
         <v>39</v>
+      </c>
+      <c r="J366" s="9" t="s">
+        <v>293</v>
       </c>
     </row>
     <row r="367" spans="1:74" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -11798,13 +11628,13 @@
     </row>
     <row r="368" spans="1:74" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A368" s="9" t="s">
-        <v>414</v>
+        <v>370</v>
       </c>
       <c r="D368" s="9" t="s">
-        <v>415</v>
+        <v>402</v>
       </c>
       <c r="I368" s="9" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
     </row>
     <row r="369" spans="1:74" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -11885,13 +11715,13 @@
     </row>
     <row r="370" spans="1:74" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A370" s="9" t="s">
-        <v>416</v>
+        <v>342</v>
       </c>
       <c r="D370" s="9" t="s">
-        <v>424</v>
+        <v>403</v>
       </c>
       <c r="I370" s="9" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
     </row>
     <row r="371" spans="1:74" s="9" customFormat="1" x14ac:dyDescent="0.2">
@@ -11972,10 +11802,10 @@
     </row>
     <row r="372" spans="1:74" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A372" s="9" t="s">
-        <v>417</v>
+        <v>371</v>
       </c>
       <c r="D372" s="9" t="s">
-        <v>425</v>
+        <v>404</v>
       </c>
       <c r="I372" s="9" t="s">
         <v>50</v>
@@ -12057,7 +11887,17 @@
       <c r="BU373" s="17"/>
       <c r="BV373" s="17"/>
     </row>
-    <row r="374" spans="1:74" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="374" spans="1:74" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A374" s="9" t="s">
+        <v>408</v>
+      </c>
+      <c r="D374" s="9" t="s">
+        <v>409</v>
+      </c>
+      <c r="I374" s="9" t="s">
+        <v>50</v>
+      </c>
+    </row>
     <row r="375" spans="1:74" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A375" s="17"/>
       <c r="B375" s="17"/>
@@ -12134,6 +11974,17 @@
       <c r="BU375" s="17"/>
       <c r="BV375" s="17"/>
     </row>
+    <row r="376" spans="1:74" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A376" s="9" t="s">
+        <v>410</v>
+      </c>
+      <c r="D376" s="9" t="s">
+        <v>411</v>
+      </c>
+      <c r="I376" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
     <row r="377" spans="1:74" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A377" s="17"/>
       <c r="B377" s="17"/>
@@ -12210,6 +12061,17 @@
       <c r="BU377" s="17"/>
       <c r="BV377" s="17"/>
     </row>
+    <row r="378" spans="1:74" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A378" s="9" t="s">
+        <v>412</v>
+      </c>
+      <c r="D378" s="9" t="s">
+        <v>413</v>
+      </c>
+      <c r="I378" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
     <row r="379" spans="1:74" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A379" s="17"/>
       <c r="B379" s="17"/>
@@ -12286,6 +12148,17 @@
       <c r="BU379" s="17"/>
       <c r="BV379" s="17"/>
     </row>
+    <row r="380" spans="1:74" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A380" s="9" t="s">
+        <v>414</v>
+      </c>
+      <c r="D380" s="9" t="s">
+        <v>422</v>
+      </c>
+      <c r="I380" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
     <row r="381" spans="1:74" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A381" s="17"/>
       <c r="B381" s="17"/>
@@ -12362,6 +12235,17 @@
       <c r="BU381" s="17"/>
       <c r="BV381" s="17"/>
     </row>
+    <row r="382" spans="1:74" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A382" s="9" t="s">
+        <v>415</v>
+      </c>
+      <c r="D382" s="9" t="s">
+        <v>423</v>
+      </c>
+      <c r="I382" s="9" t="s">
+        <v>50</v>
+      </c>
+    </row>
     <row r="383" spans="1:74" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A383" s="17"/>
       <c r="B383" s="17"/>
@@ -12438,145 +12322,386 @@
       <c r="BU383" s="17"/>
       <c r="BV383" s="17"/>
     </row>
-    <row r="428" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A428" s="12"/>
-      <c r="B428" s="12"/>
-      <c r="C428" s="12"/>
-      <c r="D428" s="12"/>
-      <c r="E428" s="12"/>
-      <c r="F428" s="12"/>
-      <c r="G428" s="12"/>
-      <c r="H428" s="12"/>
-      <c r="I428" s="12"/>
-      <c r="J428" s="12"/>
-      <c r="K428" s="12"/>
-      <c r="L428" s="12"/>
-    </row>
-    <row r="429" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A429" s="12"/>
-      <c r="B429" s="12"/>
-      <c r="C429" s="12"/>
-      <c r="D429" s="12"/>
-      <c r="E429" s="12"/>
-      <c r="F429" s="12"/>
-      <c r="G429" s="12"/>
-      <c r="H429" s="12"/>
-      <c r="I429" s="12"/>
-      <c r="J429" s="12"/>
-      <c r="K429" s="12"/>
-      <c r="L429" s="12"/>
-    </row>
-    <row r="430" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A430" s="12"/>
-      <c r="B430" s="12"/>
-      <c r="C430" s="12"/>
-      <c r="D430" s="12"/>
-      <c r="E430" s="12"/>
-      <c r="F430" s="12"/>
-      <c r="G430" s="12"/>
-      <c r="H430" s="12"/>
-      <c r="I430" s="12"/>
-      <c r="J430" s="12"/>
-      <c r="K430" s="12"/>
-      <c r="L430" s="12"/>
-    </row>
-    <row r="431" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A431" s="12"/>
-      <c r="B431" s="12"/>
-      <c r="C431" s="12"/>
-      <c r="D431" s="12"/>
-      <c r="E431" s="12"/>
-      <c r="F431" s="12"/>
-      <c r="G431" s="12"/>
-      <c r="H431" s="12"/>
-      <c r="I431" s="12"/>
-      <c r="J431" s="12"/>
-      <c r="K431" s="12"/>
-      <c r="L431" s="12"/>
-    </row>
-    <row r="432" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A432" s="14"/>
-      <c r="B432" s="14"/>
-      <c r="C432" s="14"/>
-      <c r="D432" s="14"/>
-      <c r="E432" s="14"/>
-      <c r="F432" s="14"/>
-      <c r="G432" s="14"/>
-      <c r="H432" s="14"/>
-      <c r="I432" s="14"/>
-      <c r="J432" s="14"/>
-      <c r="K432" s="12"/>
-      <c r="L432" s="12"/>
-    </row>
-    <row r="433" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A433" s="14"/>
-      <c r="B433" s="14"/>
-      <c r="C433" s="14"/>
-      <c r="D433" s="14"/>
-      <c r="E433" s="14"/>
-      <c r="F433" s="14"/>
-      <c r="G433" s="14"/>
-      <c r="H433" s="14"/>
-      <c r="I433" s="14"/>
-      <c r="J433" s="14"/>
-      <c r="K433" s="12"/>
-      <c r="L433" s="12"/>
-    </row>
-    <row r="434" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A434" s="14"/>
-      <c r="B434" s="14"/>
-      <c r="C434" s="14"/>
-      <c r="D434" s="14"/>
-      <c r="E434" s="14"/>
-      <c r="F434" s="14"/>
-      <c r="G434" s="14"/>
-      <c r="H434" s="14"/>
-      <c r="I434" s="14"/>
-      <c r="J434" s="14"/>
-      <c r="K434" s="12"/>
-      <c r="L434" s="12"/>
-    </row>
-    <row r="435" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A435" s="14"/>
-      <c r="B435" s="14"/>
-      <c r="C435" s="14"/>
-      <c r="D435" s="14"/>
-      <c r="E435" s="14"/>
-      <c r="F435" s="14"/>
-      <c r="G435" s="14"/>
-      <c r="H435" s="14"/>
-      <c r="I435" s="14"/>
-      <c r="J435" s="14"/>
-      <c r="K435" s="12"/>
-      <c r="L435" s="12"/>
-    </row>
-    <row r="436" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A436" s="14"/>
-      <c r="B436" s="14"/>
-      <c r="C436" s="14"/>
-      <c r="D436" s="14"/>
-      <c r="E436" s="14"/>
-      <c r="F436" s="14"/>
-      <c r="G436" s="14"/>
-      <c r="H436" s="14"/>
-      <c r="I436" s="14"/>
-      <c r="J436" s="14"/>
-      <c r="K436" s="12"/>
-      <c r="L436" s="12"/>
-    </row>
-    <row r="437" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A437" s="12"/>
-      <c r="B437" s="12"/>
-      <c r="C437" s="12"/>
-      <c r="D437" s="12"/>
-      <c r="E437" s="12"/>
-      <c r="F437" s="12"/>
-      <c r="G437" s="12"/>
-      <c r="H437" s="12"/>
-      <c r="I437" s="12"/>
-      <c r="J437" s="12"/>
-      <c r="K437" s="12"/>
-      <c r="L437" s="12"/>
+    <row r="384" spans="1:74" s="9" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="385" spans="1:74" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A385" s="17"/>
+      <c r="B385" s="17"/>
+      <c r="C385" s="17"/>
+      <c r="D385" s="17"/>
+      <c r="E385" s="17"/>
+      <c r="F385" s="17"/>
+      <c r="G385" s="17"/>
+      <c r="H385" s="17"/>
+      <c r="I385" s="17"/>
+      <c r="J385" s="17"/>
+      <c r="K385" s="17"/>
+      <c r="L385" s="17"/>
+      <c r="M385" s="17"/>
+      <c r="N385" s="17"/>
+      <c r="O385" s="17"/>
+      <c r="P385" s="17"/>
+      <c r="Q385" s="17"/>
+      <c r="R385" s="17"/>
+      <c r="S385" s="17"/>
+      <c r="T385" s="17"/>
+      <c r="U385" s="17"/>
+      <c r="V385" s="17"/>
+      <c r="W385" s="17"/>
+      <c r="X385" s="17"/>
+      <c r="Y385" s="17"/>
+      <c r="Z385" s="17"/>
+      <c r="AA385" s="17"/>
+      <c r="AB385" s="17"/>
+      <c r="AC385" s="17"/>
+      <c r="AD385" s="17"/>
+      <c r="AE385" s="17"/>
+      <c r="AF385" s="17"/>
+      <c r="AG385" s="17"/>
+      <c r="AH385" s="17"/>
+      <c r="AI385" s="17"/>
+      <c r="AJ385" s="17"/>
+      <c r="AK385" s="17"/>
+      <c r="AL385" s="17"/>
+      <c r="AM385" s="17"/>
+      <c r="AN385" s="17"/>
+      <c r="AO385" s="17"/>
+      <c r="AP385" s="17"/>
+      <c r="AQ385" s="17"/>
+      <c r="AR385" s="17"/>
+      <c r="AS385" s="17"/>
+      <c r="AT385" s="17"/>
+      <c r="AU385" s="17"/>
+      <c r="AV385" s="17"/>
+      <c r="AW385" s="17"/>
+      <c r="AX385" s="17"/>
+      <c r="AY385" s="17"/>
+      <c r="AZ385" s="17"/>
+      <c r="BA385" s="17"/>
+      <c r="BB385" s="17"/>
+      <c r="BC385" s="17"/>
+      <c r="BD385" s="17"/>
+      <c r="BE385" s="17"/>
+      <c r="BF385" s="17"/>
+      <c r="BG385" s="17"/>
+      <c r="BH385" s="17"/>
+      <c r="BI385" s="17"/>
+      <c r="BJ385" s="17"/>
+      <c r="BK385" s="17"/>
+      <c r="BL385" s="17"/>
+      <c r="BM385" s="17"/>
+      <c r="BN385" s="17"/>
+      <c r="BO385" s="17"/>
+      <c r="BP385" s="17"/>
+      <c r="BQ385" s="17"/>
+      <c r="BR385" s="17"/>
+      <c r="BS385" s="17"/>
+      <c r="BT385" s="17"/>
+      <c r="BU385" s="17"/>
+      <c r="BV385" s="17"/>
+    </row>
+    <row r="387" spans="1:74" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A387" s="17"/>
+      <c r="B387" s="17"/>
+      <c r="C387" s="17"/>
+      <c r="D387" s="17"/>
+      <c r="E387" s="17"/>
+      <c r="F387" s="17"/>
+      <c r="G387" s="17"/>
+      <c r="H387" s="17"/>
+      <c r="I387" s="17"/>
+      <c r="J387" s="17"/>
+      <c r="K387" s="17"/>
+      <c r="L387" s="17"/>
+      <c r="M387" s="17"/>
+      <c r="N387" s="17"/>
+      <c r="O387" s="17"/>
+      <c r="P387" s="17"/>
+      <c r="Q387" s="17"/>
+      <c r="R387" s="17"/>
+      <c r="S387" s="17"/>
+      <c r="T387" s="17"/>
+      <c r="U387" s="17"/>
+      <c r="V387" s="17"/>
+      <c r="W387" s="17"/>
+      <c r="X387" s="17"/>
+      <c r="Y387" s="17"/>
+      <c r="Z387" s="17"/>
+      <c r="AA387" s="17"/>
+      <c r="AB387" s="17"/>
+      <c r="AC387" s="17"/>
+      <c r="AD387" s="17"/>
+      <c r="AE387" s="17"/>
+      <c r="AF387" s="17"/>
+      <c r="AG387" s="17"/>
+      <c r="AH387" s="17"/>
+      <c r="AI387" s="17"/>
+      <c r="AJ387" s="17"/>
+      <c r="AK387" s="17"/>
+      <c r="AL387" s="17"/>
+      <c r="AM387" s="17"/>
+      <c r="AN387" s="17"/>
+      <c r="AO387" s="17"/>
+      <c r="AP387" s="17"/>
+      <c r="AQ387" s="17"/>
+      <c r="AR387" s="17"/>
+      <c r="AS387" s="17"/>
+      <c r="AT387" s="17"/>
+      <c r="AU387" s="17"/>
+      <c r="AV387" s="17"/>
+      <c r="AW387" s="17"/>
+      <c r="AX387" s="17"/>
+      <c r="AY387" s="17"/>
+      <c r="AZ387" s="17"/>
+      <c r="BA387" s="17"/>
+      <c r="BB387" s="17"/>
+      <c r="BC387" s="17"/>
+      <c r="BD387" s="17"/>
+      <c r="BE387" s="17"/>
+      <c r="BF387" s="17"/>
+      <c r="BG387" s="17"/>
+      <c r="BH387" s="17"/>
+      <c r="BI387" s="17"/>
+      <c r="BJ387" s="17"/>
+      <c r="BK387" s="17"/>
+      <c r="BL387" s="17"/>
+      <c r="BM387" s="17"/>
+      <c r="BN387" s="17"/>
+      <c r="BO387" s="17"/>
+      <c r="BP387" s="17"/>
+      <c r="BQ387" s="17"/>
+      <c r="BR387" s="17"/>
+      <c r="BS387" s="17"/>
+      <c r="BT387" s="17"/>
+      <c r="BU387" s="17"/>
+      <c r="BV387" s="17"/>
+    </row>
+    <row r="389" spans="1:74" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A389" s="17"/>
+      <c r="B389" s="17"/>
+      <c r="C389" s="17"/>
+      <c r="D389" s="17"/>
+      <c r="E389" s="17"/>
+      <c r="F389" s="17"/>
+      <c r="G389" s="17"/>
+      <c r="H389" s="17"/>
+      <c r="I389" s="17"/>
+      <c r="J389" s="17"/>
+      <c r="K389" s="17"/>
+      <c r="L389" s="17"/>
+      <c r="M389" s="17"/>
+      <c r="N389" s="17"/>
+      <c r="O389" s="17"/>
+      <c r="P389" s="17"/>
+      <c r="Q389" s="17"/>
+      <c r="R389" s="17"/>
+      <c r="S389" s="17"/>
+      <c r="T389" s="17"/>
+      <c r="U389" s="17"/>
+      <c r="V389" s="17"/>
+      <c r="W389" s="17"/>
+      <c r="X389" s="17"/>
+      <c r="Y389" s="17"/>
+      <c r="Z389" s="17"/>
+      <c r="AA389" s="17"/>
+      <c r="AB389" s="17"/>
+      <c r="AC389" s="17"/>
+      <c r="AD389" s="17"/>
+      <c r="AE389" s="17"/>
+      <c r="AF389" s="17"/>
+      <c r="AG389" s="17"/>
+      <c r="AH389" s="17"/>
+      <c r="AI389" s="17"/>
+      <c r="AJ389" s="17"/>
+      <c r="AK389" s="17"/>
+      <c r="AL389" s="17"/>
+      <c r="AM389" s="17"/>
+      <c r="AN389" s="17"/>
+      <c r="AO389" s="17"/>
+      <c r="AP389" s="17"/>
+      <c r="AQ389" s="17"/>
+      <c r="AR389" s="17"/>
+      <c r="AS389" s="17"/>
+      <c r="AT389" s="17"/>
+      <c r="AU389" s="17"/>
+      <c r="AV389" s="17"/>
+      <c r="AW389" s="17"/>
+      <c r="AX389" s="17"/>
+      <c r="AY389" s="17"/>
+      <c r="AZ389" s="17"/>
+      <c r="BA389" s="17"/>
+      <c r="BB389" s="17"/>
+      <c r="BC389" s="17"/>
+      <c r="BD389" s="17"/>
+      <c r="BE389" s="17"/>
+      <c r="BF389" s="17"/>
+      <c r="BG389" s="17"/>
+      <c r="BH389" s="17"/>
+      <c r="BI389" s="17"/>
+      <c r="BJ389" s="17"/>
+      <c r="BK389" s="17"/>
+      <c r="BL389" s="17"/>
+      <c r="BM389" s="17"/>
+      <c r="BN389" s="17"/>
+      <c r="BO389" s="17"/>
+      <c r="BP389" s="17"/>
+      <c r="BQ389" s="17"/>
+      <c r="BR389" s="17"/>
+      <c r="BS389" s="17"/>
+      <c r="BT389" s="17"/>
+      <c r="BU389" s="17"/>
+      <c r="BV389" s="17"/>
+    </row>
+    <row r="391" spans="1:74" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A391" s="17"/>
+      <c r="B391" s="17"/>
+      <c r="C391" s="17"/>
+      <c r="D391" s="17"/>
+      <c r="E391" s="17"/>
+      <c r="F391" s="17"/>
+      <c r="G391" s="17"/>
+      <c r="H391" s="17"/>
+      <c r="I391" s="17"/>
+      <c r="J391" s="17"/>
+      <c r="K391" s="17"/>
+      <c r="L391" s="17"/>
+      <c r="M391" s="17"/>
+      <c r="N391" s="17"/>
+      <c r="O391" s="17"/>
+      <c r="P391" s="17"/>
+      <c r="Q391" s="17"/>
+      <c r="R391" s="17"/>
+      <c r="S391" s="17"/>
+      <c r="T391" s="17"/>
+      <c r="U391" s="17"/>
+      <c r="V391" s="17"/>
+      <c r="W391" s="17"/>
+      <c r="X391" s="17"/>
+      <c r="Y391" s="17"/>
+      <c r="Z391" s="17"/>
+      <c r="AA391" s="17"/>
+      <c r="AB391" s="17"/>
+      <c r="AC391" s="17"/>
+      <c r="AD391" s="17"/>
+      <c r="AE391" s="17"/>
+      <c r="AF391" s="17"/>
+      <c r="AG391" s="17"/>
+      <c r="AH391" s="17"/>
+      <c r="AI391" s="17"/>
+      <c r="AJ391" s="17"/>
+      <c r="AK391" s="17"/>
+      <c r="AL391" s="17"/>
+      <c r="AM391" s="17"/>
+      <c r="AN391" s="17"/>
+      <c r="AO391" s="17"/>
+      <c r="AP391" s="17"/>
+      <c r="AQ391" s="17"/>
+      <c r="AR391" s="17"/>
+      <c r="AS391" s="17"/>
+      <c r="AT391" s="17"/>
+      <c r="AU391" s="17"/>
+      <c r="AV391" s="17"/>
+      <c r="AW391" s="17"/>
+      <c r="AX391" s="17"/>
+      <c r="AY391" s="17"/>
+      <c r="AZ391" s="17"/>
+      <c r="BA391" s="17"/>
+      <c r="BB391" s="17"/>
+      <c r="BC391" s="17"/>
+      <c r="BD391" s="17"/>
+      <c r="BE391" s="17"/>
+      <c r="BF391" s="17"/>
+      <c r="BG391" s="17"/>
+      <c r="BH391" s="17"/>
+      <c r="BI391" s="17"/>
+      <c r="BJ391" s="17"/>
+      <c r="BK391" s="17"/>
+      <c r="BL391" s="17"/>
+      <c r="BM391" s="17"/>
+      <c r="BN391" s="17"/>
+      <c r="BO391" s="17"/>
+      <c r="BP391" s="17"/>
+      <c r="BQ391" s="17"/>
+      <c r="BR391" s="17"/>
+      <c r="BS391" s="17"/>
+      <c r="BT391" s="17"/>
+      <c r="BU391" s="17"/>
+      <c r="BV391" s="17"/>
+    </row>
+    <row r="393" spans="1:74" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A393" s="17"/>
+      <c r="B393" s="17"/>
+      <c r="C393" s="17"/>
+      <c r="D393" s="17"/>
+      <c r="E393" s="17"/>
+      <c r="F393" s="17"/>
+      <c r="G393" s="17"/>
+      <c r="H393" s="17"/>
+      <c r="I393" s="17"/>
+      <c r="J393" s="17"/>
+      <c r="K393" s="17"/>
+      <c r="L393" s="17"/>
+      <c r="M393" s="17"/>
+      <c r="N393" s="17"/>
+      <c r="O393" s="17"/>
+      <c r="P393" s="17"/>
+      <c r="Q393" s="17"/>
+      <c r="R393" s="17"/>
+      <c r="S393" s="17"/>
+      <c r="T393" s="17"/>
+      <c r="U393" s="17"/>
+      <c r="V393" s="17"/>
+      <c r="W393" s="17"/>
+      <c r="X393" s="17"/>
+      <c r="Y393" s="17"/>
+      <c r="Z393" s="17"/>
+      <c r="AA393" s="17"/>
+      <c r="AB393" s="17"/>
+      <c r="AC393" s="17"/>
+      <c r="AD393" s="17"/>
+      <c r="AE393" s="17"/>
+      <c r="AF393" s="17"/>
+      <c r="AG393" s="17"/>
+      <c r="AH393" s="17"/>
+      <c r="AI393" s="17"/>
+      <c r="AJ393" s="17"/>
+      <c r="AK393" s="17"/>
+      <c r="AL393" s="17"/>
+      <c r="AM393" s="17"/>
+      <c r="AN393" s="17"/>
+      <c r="AO393" s="17"/>
+      <c r="AP393" s="17"/>
+      <c r="AQ393" s="17"/>
+      <c r="AR393" s="17"/>
+      <c r="AS393" s="17"/>
+      <c r="AT393" s="17"/>
+      <c r="AU393" s="17"/>
+      <c r="AV393" s="17"/>
+      <c r="AW393" s="17"/>
+      <c r="AX393" s="17"/>
+      <c r="AY393" s="17"/>
+      <c r="AZ393" s="17"/>
+      <c r="BA393" s="17"/>
+      <c r="BB393" s="17"/>
+      <c r="BC393" s="17"/>
+      <c r="BD393" s="17"/>
+      <c r="BE393" s="17"/>
+      <c r="BF393" s="17"/>
+      <c r="BG393" s="17"/>
+      <c r="BH393" s="17"/>
+      <c r="BI393" s="17"/>
+      <c r="BJ393" s="17"/>
+      <c r="BK393" s="17"/>
+      <c r="BL393" s="17"/>
+      <c r="BM393" s="17"/>
+      <c r="BN393" s="17"/>
+      <c r="BO393" s="17"/>
+      <c r="BP393" s="17"/>
+      <c r="BQ393" s="17"/>
+      <c r="BR393" s="17"/>
+      <c r="BS393" s="17"/>
+      <c r="BT393" s="17"/>
+      <c r="BU393" s="17"/>
+      <c r="BV393" s="17"/>
     </row>
     <row r="438" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A438" s="12"/>
@@ -12620,17 +12745,17 @@
       <c r="K440" s="12"/>
       <c r="L440" s="12"/>
     </row>
-    <row r="441" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A441" s="14"/>
-      <c r="B441" s="14"/>
-      <c r="C441" s="14"/>
-      <c r="D441" s="14"/>
-      <c r="E441" s="14"/>
-      <c r="F441" s="14"/>
-      <c r="G441" s="14"/>
-      <c r="H441" s="14"/>
-      <c r="I441" s="14"/>
-      <c r="J441" s="14"/>
+    <row r="441" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A441" s="12"/>
+      <c r="B441" s="12"/>
+      <c r="C441" s="12"/>
+      <c r="D441" s="12"/>
+      <c r="E441" s="12"/>
+      <c r="F441" s="12"/>
+      <c r="G441" s="12"/>
+      <c r="H441" s="12"/>
+      <c r="I441" s="12"/>
+      <c r="J441" s="12"/>
       <c r="K441" s="12"/>
       <c r="L441" s="12"/>
     </row>
@@ -12704,45 +12829,45 @@
       <c r="K446" s="12"/>
       <c r="L446" s="12"/>
     </row>
-    <row r="447" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A447" s="14"/>
-      <c r="B447" s="14"/>
-      <c r="C447" s="14"/>
-      <c r="D447" s="14"/>
-      <c r="E447" s="14"/>
-      <c r="F447" s="14"/>
-      <c r="G447" s="14"/>
-      <c r="H447" s="14"/>
-      <c r="I447" s="14"/>
-      <c r="J447" s="14"/>
+    <row r="447" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A447" s="12"/>
+      <c r="B447" s="12"/>
+      <c r="C447" s="12"/>
+      <c r="D447" s="12"/>
+      <c r="E447" s="12"/>
+      <c r="F447" s="12"/>
+      <c r="G447" s="12"/>
+      <c r="H447" s="12"/>
+      <c r="I447" s="12"/>
+      <c r="J447" s="12"/>
       <c r="K447" s="12"/>
       <c r="L447" s="12"/>
     </row>
-    <row r="448" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A448" s="14"/>
-      <c r="B448" s="14"/>
-      <c r="C448" s="14"/>
-      <c r="D448" s="14"/>
-      <c r="E448" s="14"/>
-      <c r="F448" s="14"/>
-      <c r="G448" s="14"/>
-      <c r="H448" s="14"/>
-      <c r="I448" s="14"/>
-      <c r="J448" s="14"/>
+    <row r="448" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A448" s="12"/>
+      <c r="B448" s="12"/>
+      <c r="C448" s="12"/>
+      <c r="D448" s="12"/>
+      <c r="E448" s="12"/>
+      <c r="F448" s="12"/>
+      <c r="G448" s="12"/>
+      <c r="H448" s="12"/>
+      <c r="I448" s="12"/>
+      <c r="J448" s="12"/>
       <c r="K448" s="12"/>
       <c r="L448" s="12"/>
     </row>
-    <row r="449" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A449" s="14"/>
-      <c r="B449" s="14"/>
-      <c r="C449" s="14"/>
-      <c r="D449" s="14"/>
-      <c r="E449" s="14"/>
-      <c r="F449" s="14"/>
-      <c r="G449" s="14"/>
-      <c r="H449" s="14"/>
-      <c r="I449" s="14"/>
-      <c r="J449" s="14"/>
+    <row r="449" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A449" s="12"/>
+      <c r="B449" s="12"/>
+      <c r="C449" s="12"/>
+      <c r="D449" s="12"/>
+      <c r="E449" s="12"/>
+      <c r="F449" s="12"/>
+      <c r="G449" s="12"/>
+      <c r="H449" s="12"/>
+      <c r="I449" s="12"/>
+      <c r="J449" s="12"/>
       <c r="K449" s="12"/>
       <c r="L449" s="12"/>
     </row>
@@ -12760,31 +12885,31 @@
       <c r="K450" s="12"/>
       <c r="L450" s="12"/>
     </row>
-    <row r="451" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A451" s="12"/>
-      <c r="B451" s="12"/>
-      <c r="C451" s="12"/>
-      <c r="D451" s="12"/>
-      <c r="E451" s="12"/>
-      <c r="F451" s="12"/>
-      <c r="G451" s="12"/>
-      <c r="H451" s="12"/>
-      <c r="I451" s="12"/>
-      <c r="J451" s="12"/>
+    <row r="451" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A451" s="14"/>
+      <c r="B451" s="14"/>
+      <c r="C451" s="14"/>
+      <c r="D451" s="14"/>
+      <c r="E451" s="14"/>
+      <c r="F451" s="14"/>
+      <c r="G451" s="14"/>
+      <c r="H451" s="14"/>
+      <c r="I451" s="14"/>
+      <c r="J451" s="14"/>
       <c r="K451" s="12"/>
       <c r="L451" s="12"/>
     </row>
-    <row r="452" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A452" s="12"/>
-      <c r="B452" s="12"/>
-      <c r="C452" s="12"/>
-      <c r="D452" s="12"/>
-      <c r="E452" s="12"/>
-      <c r="F452" s="12"/>
-      <c r="G452" s="12"/>
-      <c r="H452" s="12"/>
-      <c r="I452" s="12"/>
-      <c r="J452" s="12"/>
+    <row r="452" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A452" s="14"/>
+      <c r="B452" s="14"/>
+      <c r="C452" s="14"/>
+      <c r="D452" s="14"/>
+      <c r="E452" s="14"/>
+      <c r="F452" s="14"/>
+      <c r="G452" s="14"/>
+      <c r="H452" s="14"/>
+      <c r="I452" s="14"/>
+      <c r="J452" s="14"/>
       <c r="K452" s="12"/>
       <c r="L452" s="12"/>
     </row>
@@ -12886,59 +13011,59 @@
       <c r="K459" s="12"/>
       <c r="L459" s="12"/>
     </row>
-    <row r="460" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="460" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A460" s="12"/>
       <c r="B460" s="12"/>
       <c r="C460" s="12"/>
       <c r="D460" s="12"/>
       <c r="E460" s="12"/>
       <c r="F460" s="12"/>
-      <c r="G460" s="14"/>
-      <c r="H460" s="14"/>
-      <c r="I460" s="14"/>
-      <c r="J460" s="14"/>
+      <c r="G460" s="12"/>
+      <c r="H460" s="12"/>
+      <c r="I460" s="12"/>
+      <c r="J460" s="12"/>
       <c r="K460" s="12"/>
       <c r="L460" s="12"/>
     </row>
-    <row r="461" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="461" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A461" s="12"/>
       <c r="B461" s="12"/>
       <c r="C461" s="12"/>
       <c r="D461" s="12"/>
       <c r="E461" s="12"/>
       <c r="F461" s="12"/>
-      <c r="G461" s="14"/>
-      <c r="H461" s="14"/>
-      <c r="I461" s="14"/>
-      <c r="J461" s="14"/>
+      <c r="G461" s="12"/>
+      <c r="H461" s="12"/>
+      <c r="I461" s="12"/>
+      <c r="J461" s="12"/>
       <c r="K461" s="12"/>
       <c r="L461" s="12"/>
     </row>
-    <row r="462" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="462" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A462" s="12"/>
       <c r="B462" s="12"/>
       <c r="C462" s="12"/>
       <c r="D462" s="12"/>
       <c r="E462" s="12"/>
       <c r="F462" s="12"/>
-      <c r="G462" s="14"/>
-      <c r="H462" s="14"/>
-      <c r="I462" s="14"/>
-      <c r="J462" s="14"/>
+      <c r="G462" s="12"/>
+      <c r="H462" s="12"/>
+      <c r="I462" s="12"/>
+      <c r="J462" s="12"/>
       <c r="K462" s="12"/>
       <c r="L462" s="12"/>
     </row>
-    <row r="463" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A463" s="12"/>
-      <c r="B463" s="12"/>
-      <c r="C463" s="12"/>
-      <c r="D463" s="12"/>
-      <c r="E463" s="12"/>
-      <c r="F463" s="12"/>
-      <c r="G463" s="12"/>
-      <c r="H463" s="12"/>
-      <c r="I463" s="12"/>
-      <c r="J463" s="12"/>
+    <row r="463" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A463" s="14"/>
+      <c r="B463" s="14"/>
+      <c r="C463" s="14"/>
+      <c r="D463" s="14"/>
+      <c r="E463" s="14"/>
+      <c r="F463" s="14"/>
+      <c r="G463" s="14"/>
+      <c r="H463" s="14"/>
+      <c r="I463" s="14"/>
+      <c r="J463" s="14"/>
       <c r="K463" s="12"/>
       <c r="L463" s="12"/>
     </row>
@@ -12970,40 +13095,180 @@
       <c r="K465" s="12"/>
       <c r="L465" s="12"/>
     </row>
-    <row r="490" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A490" s="9"/>
-      <c r="B490" s="9"/>
-      <c r="C490" s="9"/>
-      <c r="D490" s="9"/>
-      <c r="E490" s="9"/>
-      <c r="F490" s="9"/>
-      <c r="G490" s="9"/>
-      <c r="H490" s="9"/>
-      <c r="I490" s="9"/>
-      <c r="J490" s="9"/>
-    </row>
-    <row r="492" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A492" t="s">
+    <row r="466" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A466" s="14"/>
+      <c r="B466" s="14"/>
+      <c r="C466" s="14"/>
+      <c r="D466" s="14"/>
+      <c r="E466" s="14"/>
+      <c r="F466" s="14"/>
+      <c r="G466" s="14"/>
+      <c r="H466" s="14"/>
+      <c r="I466" s="14"/>
+      <c r="J466" s="14"/>
+      <c r="K466" s="12"/>
+      <c r="L466" s="12"/>
+    </row>
+    <row r="467" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A467" s="14"/>
+      <c r="B467" s="14"/>
+      <c r="C467" s="14"/>
+      <c r="D467" s="14"/>
+      <c r="E467" s="14"/>
+      <c r="F467" s="14"/>
+      <c r="G467" s="14"/>
+      <c r="H467" s="14"/>
+      <c r="I467" s="14"/>
+      <c r="J467" s="14"/>
+      <c r="K467" s="12"/>
+      <c r="L467" s="12"/>
+    </row>
+    <row r="468" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A468" s="14"/>
+      <c r="B468" s="14"/>
+      <c r="C468" s="14"/>
+      <c r="D468" s="14"/>
+      <c r="E468" s="14"/>
+      <c r="F468" s="14"/>
+      <c r="G468" s="14"/>
+      <c r="H468" s="14"/>
+      <c r="I468" s="14"/>
+      <c r="J468" s="14"/>
+      <c r="K468" s="12"/>
+      <c r="L468" s="12"/>
+    </row>
+    <row r="469" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A469" s="14"/>
+      <c r="B469" s="14"/>
+      <c r="C469" s="14"/>
+      <c r="D469" s="14"/>
+      <c r="E469" s="14"/>
+      <c r="F469" s="14"/>
+      <c r="G469" s="14"/>
+      <c r="H469" s="14"/>
+      <c r="I469" s="14"/>
+      <c r="J469" s="14"/>
+      <c r="K469" s="12"/>
+      <c r="L469" s="12"/>
+    </row>
+    <row r="470" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A470" s="12"/>
+      <c r="B470" s="12"/>
+      <c r="C470" s="12"/>
+      <c r="D470" s="12"/>
+      <c r="E470" s="12"/>
+      <c r="F470" s="12"/>
+      <c r="G470" s="14"/>
+      <c r="H470" s="14"/>
+      <c r="I470" s="14"/>
+      <c r="J470" s="14"/>
+      <c r="K470" s="12"/>
+      <c r="L470" s="12"/>
+    </row>
+    <row r="471" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A471" s="12"/>
+      <c r="B471" s="12"/>
+      <c r="C471" s="12"/>
+      <c r="D471" s="12"/>
+      <c r="E471" s="12"/>
+      <c r="F471" s="12"/>
+      <c r="G471" s="14"/>
+      <c r="H471" s="14"/>
+      <c r="I471" s="14"/>
+      <c r="J471" s="14"/>
+      <c r="K471" s="12"/>
+      <c r="L471" s="12"/>
+    </row>
+    <row r="472" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A472" s="12"/>
+      <c r="B472" s="12"/>
+      <c r="C472" s="12"/>
+      <c r="D472" s="12"/>
+      <c r="E472" s="12"/>
+      <c r="F472" s="12"/>
+      <c r="G472" s="14"/>
+      <c r="H472" s="14"/>
+      <c r="I472" s="14"/>
+      <c r="J472" s="14"/>
+      <c r="K472" s="12"/>
+      <c r="L472" s="12"/>
+    </row>
+    <row r="473" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A473" s="12"/>
+      <c r="B473" s="12"/>
+      <c r="C473" s="12"/>
+      <c r="D473" s="12"/>
+      <c r="E473" s="12"/>
+      <c r="F473" s="12"/>
+      <c r="G473" s="12"/>
+      <c r="H473" s="12"/>
+      <c r="I473" s="12"/>
+      <c r="J473" s="12"/>
+      <c r="K473" s="12"/>
+      <c r="L473" s="12"/>
+    </row>
+    <row r="474" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A474" s="14"/>
+      <c r="B474" s="14"/>
+      <c r="C474" s="14"/>
+      <c r="D474" s="14"/>
+      <c r="E474" s="14"/>
+      <c r="F474" s="14"/>
+      <c r="G474" s="14"/>
+      <c r="H474" s="14"/>
+      <c r="I474" s="14"/>
+      <c r="J474" s="14"/>
+      <c r="K474" s="12"/>
+      <c r="L474" s="12"/>
+    </row>
+    <row r="475" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A475" s="14"/>
+      <c r="B475" s="14"/>
+      <c r="C475" s="14"/>
+      <c r="D475" s="14"/>
+      <c r="E475" s="14"/>
+      <c r="F475" s="14"/>
+      <c r="G475" s="14"/>
+      <c r="H475" s="14"/>
+      <c r="I475" s="14"/>
+      <c r="J475" s="14"/>
+      <c r="K475" s="12"/>
+      <c r="L475" s="12"/>
+    </row>
+    <row r="500" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A500" s="9"/>
+      <c r="B500" s="9"/>
+      <c r="C500" s="9"/>
+      <c r="D500" s="9"/>
+      <c r="E500" s="9"/>
+      <c r="F500" s="9"/>
+      <c r="G500" s="9"/>
+      <c r="H500" s="9"/>
+      <c r="I500" s="9"/>
+      <c r="J500" s="9"/>
+    </row>
+    <row r="502" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A502" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="493" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A493" t="s">
+    <row r="503" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A503" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="494" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A494" t="s">
+    <row r="504" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A504" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="495" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A495" t="s">
+    <row r="505" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A505" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="496" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A496" t="s">
+    <row r="506" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A506" t="s">
         <v>125</v>
       </c>
     </row>

</xml_diff>